<commit_message>
Spreadsheet for recording MCMC values
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Belgium</t>
   </si>
@@ -50,7 +50,25 @@
     <t>ESS</t>
   </si>
   <si>
-    <t>param0</t>
+    <t>Starting values</t>
+  </si>
+  <si>
+    <t>gamma0</t>
+  </si>
+  <si>
+    <t>gamma1</t>
+  </si>
+  <si>
+    <t>File names</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Prop. fac.</t>
   </si>
 </sst>
 </file>
@@ -94,16 +112,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,77 +403,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" t="s">
-        <v>8</v>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>0.2</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>1E-3</v>
       </c>
-      <c r="E3" s="1">
+      <c r="H3" s="1">
         <v>2000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="I3" s="3">
         <v>0.29799999999999999</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>255</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="G1:H1"/>
+  <mergeCells count="3">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated settings for BE loglin
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Belgium</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Prop. fac.</t>
+  </si>
+  <si>
+    <t>loglin</t>
   </si>
 </sst>
 </file>
@@ -115,14 +118,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,20 +406,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -427,86 +430,164 @@
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>0.05</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>0.2</v>
       </c>
-      <c r="G3">
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
         <v>1E-3</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J4" s="1">
         <v>2000</v>
       </c>
-      <c r="I3" s="3">
+      <c r="K4" s="2">
         <v>0.29799999999999999</v>
       </c>
-      <c r="J3">
+      <c r="L4">
         <v>255</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-0.1</v>
+      </c>
+      <c r="E5">
+        <v>-3</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>-0.1</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>1E-3</v>
+      </c>
+      <c r="J5">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="L5">
+        <v>18</v>
+      </c>
+      <c r="M5">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="5">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added results of various runs
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjohnson\Documents\GitHub\HerpesZosterModel\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\HerpesZosterModel\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>Belgium</t>
   </si>
@@ -72,13 +72,25 @@
   </si>
   <si>
     <t>loglin</t>
+  </si>
+  <si>
+    <t>extloglin</t>
+  </si>
+  <si>
+    <t>gamma2</t>
+  </si>
+  <si>
+    <t>init.scale.sd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +100,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,10 +131,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -126,9 +146,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -406,50 +432,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -458,48 +488,66 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -512,35 +560,47 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>0.2</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4">
         <v>1E-3</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>2000</v>
       </c>
-      <c r="K4" s="2">
+      <c r="N4" s="2">
         <v>0.29799999999999999</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>255</v>
       </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -553,41 +613,483 @@
       <c r="D5">
         <v>-0.1</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
         <v>-3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>-1</v>
       </c>
-      <c r="G5">
-        <v>-0.1</v>
-      </c>
       <c r="H5">
+        <v>-0.1</v>
+      </c>
+      <c r="I5">
         <v>0.1</v>
       </c>
-      <c r="I5">
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5">
         <v>1E-3</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>2000</v>
       </c>
-      <c r="K5" s="5">
+      <c r="N5" s="5">
         <v>0.21</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>18</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>18</v>
       </c>
+      <c r="Q5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L7" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>-1.5</v>
+      </c>
+      <c r="D8">
+        <v>-0.05</v>
+      </c>
+      <c r="E8">
+        <v>-0.25</v>
+      </c>
+      <c r="F8">
+        <v>-2</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>-0.1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>-0.5</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0.01</v>
+      </c>
+      <c r="M8">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="O8">
+        <v>66.404989999999998</v>
+      </c>
+      <c r="P8">
+        <v>62.142000000000003</v>
+      </c>
+      <c r="Q8">
+        <v>56.486499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>-1.5</v>
+      </c>
+      <c r="D9">
+        <v>-0.05</v>
+      </c>
+      <c r="E9">
+        <v>-0.25</v>
+      </c>
+      <c r="F9">
+        <v>-2</v>
+      </c>
+      <c r="G9">
+        <v>-1.5</v>
+      </c>
+      <c r="H9">
+        <v>-0.1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>-0.1</v>
+      </c>
+      <c r="K9">
+        <v>0.1</v>
+      </c>
+      <c r="L9">
+        <v>0.01</v>
+      </c>
+      <c r="M9">
+        <v>2000</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O9">
+        <v>124.1626</v>
+      </c>
+      <c r="P9">
+        <v>128.38419999999999</v>
+      </c>
+      <c r="Q9">
+        <v>139.61969999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>-1.7</v>
+      </c>
+      <c r="D10">
+        <v>-0.03</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>-2</v>
+      </c>
+      <c r="G10">
+        <v>-1.5</v>
+      </c>
+      <c r="H10">
+        <v>-0.1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>-0.1</v>
+      </c>
+      <c r="K10">
+        <v>0.1</v>
+      </c>
+      <c r="L10">
+        <v>0.01</v>
+      </c>
+      <c r="M10">
+        <v>2000</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="O10">
+        <v>94.651880000000006</v>
+      </c>
+      <c r="P10">
+        <v>96.072630000000004</v>
+      </c>
+      <c r="Q10">
+        <v>79.661850000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>-1.5</v>
+      </c>
+      <c r="D11">
+        <v>-0.05</v>
+      </c>
+      <c r="E11">
+        <v>-0.25</v>
+      </c>
+      <c r="F11">
+        <v>-2</v>
+      </c>
+      <c r="G11">
+        <v>-1.5</v>
+      </c>
+      <c r="H11">
+        <v>-0.1</v>
+      </c>
+      <c r="I11">
+        <v>0.1</v>
+      </c>
+      <c r="J11">
+        <v>-0.1</v>
+      </c>
+      <c r="K11">
+        <v>0.1</v>
+      </c>
+      <c r="L11">
+        <v>0.01</v>
+      </c>
+      <c r="M11">
+        <v>2000</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="O11">
+        <v>123.7658</v>
+      </c>
+      <c r="P11">
+        <v>146.19380000000001</v>
+      </c>
+      <c r="Q11">
+        <v>132.3364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>-1.5</v>
+      </c>
+      <c r="D12">
+        <v>-0.05</v>
+      </c>
+      <c r="E12">
+        <v>-0.25</v>
+      </c>
+      <c r="F12">
+        <v>-1.9</v>
+      </c>
+      <c r="G12">
+        <v>-1.6</v>
+      </c>
+      <c r="H12">
+        <v>-0.1</v>
+      </c>
+      <c r="I12">
+        <v>0.1</v>
+      </c>
+      <c r="J12">
+        <v>-0.1</v>
+      </c>
+      <c r="K12">
+        <v>0.1</v>
+      </c>
+      <c r="L12">
+        <v>0.01</v>
+      </c>
+      <c r="M12">
+        <v>2000</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="O12">
+        <v>122.751</v>
+      </c>
+      <c r="P12">
+        <v>151.02969999999999</v>
+      </c>
+      <c r="Q12">
+        <v>115.8591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>-1.5</v>
+      </c>
+      <c r="D13">
+        <v>-0.05</v>
+      </c>
+      <c r="E13">
+        <v>-0.25</v>
+      </c>
+      <c r="F13">
+        <v>-1.9</v>
+      </c>
+      <c r="G13">
+        <v>-1.6</v>
+      </c>
+      <c r="H13">
+        <v>-0.05</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.1</v>
+      </c>
+      <c r="L13">
+        <v>0.01</v>
+      </c>
+      <c r="M13">
+        <v>2000</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="O13">
+        <v>147.4735</v>
+      </c>
+      <c r="P13">
+        <v>172.30279999999999</v>
+      </c>
+      <c r="Q13">
+        <v>222.35339999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>-1.5</v>
+      </c>
+      <c r="D14">
+        <v>-0.05</v>
+      </c>
+      <c r="E14">
+        <v>-0.25</v>
+      </c>
+      <c r="F14">
+        <v>-1.9</v>
+      </c>
+      <c r="G14">
+        <v>-1.8</v>
+      </c>
+      <c r="H14">
+        <v>-0.05</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>-0.1</v>
+      </c>
+      <c r="K14">
+        <v>0.1</v>
+      </c>
+      <c r="L14">
+        <v>0.01</v>
+      </c>
+      <c r="M14">
+        <v>2000</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0.35949999999999999</v>
+      </c>
+      <c r="O14">
+        <v>205.1311</v>
+      </c>
+      <c r="P14">
+        <v>204.77430000000001</v>
+      </c>
+      <c r="Q14">
+        <v>212.88749999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>-1.5</v>
+      </c>
+      <c r="D15">
+        <v>-0.05</v>
+      </c>
+      <c r="E15">
+        <v>-0.25</v>
+      </c>
+      <c r="F15">
+        <v>-1.9</v>
+      </c>
+      <c r="G15">
+        <v>-1.8</v>
+      </c>
+      <c r="H15">
+        <v>-0.05</v>
+      </c>
+      <c r="I15">
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <v>-0.1</v>
+      </c>
+      <c r="K15">
+        <v>0.05</v>
+      </c>
+      <c r="L15">
+        <v>0.01</v>
+      </c>
+      <c r="M15">
+        <v>2000</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="O15">
+        <v>150.15469999999999</v>
+      </c>
+      <c r="P15">
+        <v>245.08179999999999</v>
+      </c>
+      <c r="Q15">
+        <v>209.4426</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
+  <mergeCells count="6">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added values from this morning
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
   <si>
     <t>Belgium</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>init.scale.sd</t>
+  </si>
+  <si>
+    <t>adapt.shape.start</t>
+  </si>
+  <si>
+    <t>adapt.size.start</t>
   </si>
 </sst>
 </file>
@@ -88,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -135,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -149,8 +155,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,54 +442,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -490,33 +503,35 @@
       <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="9"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -541,13 +556,15 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="4"/>
+      <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="4"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -587,20 +604,22 @@
       <c r="M4" s="1">
         <v>2000</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2">
         <v>0.29799999999999999</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>255</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -640,25 +659,31 @@
       <c r="M5">
         <v>2000</v>
       </c>
-      <c r="N5" s="5">
+      <c r="P5" s="5">
         <v>0.21</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>18</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>18</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L7" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -698,20 +723,26 @@
       <c r="M8">
         <v>2000</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>75</v>
+      </c>
+      <c r="P8" s="7">
         <v>0.18099999999999999</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>66.404989999999998</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>62.142000000000003</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>56.486499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -751,20 +782,26 @@
       <c r="M9">
         <v>2000</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9">
+        <v>100</v>
+      </c>
+      <c r="O9">
+        <v>75</v>
+      </c>
+      <c r="P9" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>124.1626</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>128.38419999999999</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>139.61969999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -804,20 +841,26 @@
       <c r="M10">
         <v>2000</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10">
+        <v>75</v>
+      </c>
+      <c r="P10" s="7">
         <v>0.30099999999999999</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>94.651880000000006</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>96.072630000000004</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>79.661850000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -857,20 +900,26 @@
       <c r="M11">
         <v>2000</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>75</v>
+      </c>
+      <c r="P11" s="7">
         <v>0.30199999999999999</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>123.7658</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>146.19380000000001</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>132.3364</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -910,20 +959,26 @@
       <c r="M12">
         <v>2000</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>75</v>
+      </c>
+      <c r="P12" s="7">
         <v>0.29199999999999998</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>122.751</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>151.02969999999999</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>115.8591</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -963,20 +1018,26 @@
       <c r="M13">
         <v>2000</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="O13">
+        <v>75</v>
+      </c>
+      <c r="P13" s="7">
         <v>0.33750000000000002</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>147.4735</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>172.30279999999999</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>222.35339999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1016,20 +1077,26 @@
       <c r="M14">
         <v>2000</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14">
+        <v>100</v>
+      </c>
+      <c r="O14">
+        <v>75</v>
+      </c>
+      <c r="P14" s="7">
         <v>0.35949999999999999</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>205.1311</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>204.77430000000001</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>212.88749999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1069,27 +1136,398 @@
       <c r="M15">
         <v>2000</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15">
+        <v>75</v>
+      </c>
+      <c r="P15" s="7">
         <v>0.42599999999999999</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>150.15469999999999</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>245.08179999999999</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>209.4426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>-1.5</v>
+      </c>
+      <c r="D17">
+        <v>-0.05</v>
+      </c>
+      <c r="E17">
+        <v>-0.25</v>
+      </c>
+      <c r="F17">
+        <v>-2.5</v>
+      </c>
+      <c r="G17">
+        <v>-0.5</v>
+      </c>
+      <c r="H17">
+        <v>-0.1</v>
+      </c>
+      <c r="I17">
+        <v>0.05</v>
+      </c>
+      <c r="J17">
+        <v>-0.2</v>
+      </c>
+      <c r="K17">
+        <v>0.2</v>
+      </c>
+      <c r="L17">
+        <v>0.01</v>
+      </c>
+      <c r="M17">
+        <v>2000</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
+      <c r="O17">
+        <v>75</v>
+      </c>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>-1.5</v>
+      </c>
+      <c r="D18">
+        <v>-0.05</v>
+      </c>
+      <c r="E18">
+        <v>-0.25</v>
+      </c>
+      <c r="F18">
+        <v>-2.5</v>
+      </c>
+      <c r="G18">
+        <v>-1</v>
+      </c>
+      <c r="H18">
+        <v>-0.1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>-0.15</v>
+      </c>
+      <c r="K18">
+        <v>0.15</v>
+      </c>
+      <c r="L18">
+        <v>0.01</v>
+      </c>
+      <c r="M18">
+        <v>2000</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18">
+        <v>75</v>
+      </c>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>-1.5</v>
+      </c>
+      <c r="D19">
+        <v>-0.05</v>
+      </c>
+      <c r="E19">
+        <v>-0.25</v>
+      </c>
+      <c r="F19">
+        <v>-2.5</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19">
+        <v>-0.1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>-0.15</v>
+      </c>
+      <c r="K19">
+        <v>0.15</v>
+      </c>
+      <c r="L19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M19">
+        <v>2000</v>
+      </c>
+      <c r="N19">
+        <v>200</v>
+      </c>
+      <c r="O19">
+        <v>100</v>
+      </c>
+      <c r="P19" s="7">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>-1.5</v>
+      </c>
+      <c r="D21">
+        <v>-0.05</v>
+      </c>
+      <c r="E21">
+        <v>-0.25</v>
+      </c>
+      <c r="F21">
+        <v>-2.5</v>
+      </c>
+      <c r="G21">
+        <v>-1.5</v>
+      </c>
+      <c r="H21">
+        <v>-0.1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>-0.1</v>
+      </c>
+      <c r="K21">
+        <v>0.1</v>
+      </c>
+      <c r="L21">
+        <v>0.01</v>
+      </c>
+      <c r="M21">
+        <v>2000</v>
+      </c>
+      <c r="N21">
+        <v>200</v>
+      </c>
+      <c r="O21">
+        <v>100</v>
+      </c>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>-1.75</v>
+      </c>
+      <c r="D22">
+        <v>-0.05</v>
+      </c>
+      <c r="E22">
+        <v>-0.05</v>
+      </c>
+      <c r="F22">
+        <v>-2.5</v>
+      </c>
+      <c r="G22">
+        <v>-1</v>
+      </c>
+      <c r="H22">
+        <v>-0.1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>-0.1</v>
+      </c>
+      <c r="K22">
+        <v>0.1</v>
+      </c>
+      <c r="L22">
+        <v>0.01</v>
+      </c>
+      <c r="M22">
+        <v>2000</v>
+      </c>
+      <c r="N22">
+        <v>200</v>
+      </c>
+      <c r="O22">
+        <v>100</v>
+      </c>
+      <c r="P22" s="7">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="Q22">
+        <v>42.790819999999997</v>
+      </c>
+      <c r="R22">
+        <v>57.035820000000001</v>
+      </c>
+      <c r="S22">
+        <v>54.978209999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>-1.75</v>
+      </c>
+      <c r="D23">
+        <v>-0.05</v>
+      </c>
+      <c r="E23">
+        <v>-0.05</v>
+      </c>
+      <c r="F23">
+        <v>-2.5</v>
+      </c>
+      <c r="G23">
+        <v>-1</v>
+      </c>
+      <c r="H23">
+        <v>-0.1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>-0.1</v>
+      </c>
+      <c r="K23">
+        <v>0.1</v>
+      </c>
+      <c r="L23">
+        <v>0.01</v>
+      </c>
+      <c r="M23">
+        <v>2000</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23">
+        <v>75</v>
+      </c>
+      <c r="P23" s="7">
+        <v>0.219</v>
+      </c>
+      <c r="Q23">
+        <v>60.325539999999997</v>
+      </c>
+      <c r="R23">
+        <v>60.738010000000003</v>
+      </c>
+      <c r="S23">
+        <v>60.348730000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>-1.75</v>
+      </c>
+      <c r="D24">
+        <v>-0.05</v>
+      </c>
+      <c r="E24">
+        <v>-0.05</v>
+      </c>
+      <c r="F24">
+        <v>-2.5</v>
+      </c>
+      <c r="G24">
+        <v>-1</v>
+      </c>
+      <c r="H24">
+        <v>-0.1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>-0.1</v>
+      </c>
+      <c r="K24">
+        <v>0.1</v>
+      </c>
+      <c r="L24">
+        <v>0.01</v>
+      </c>
+      <c r="M24">
+        <v>5000</v>
+      </c>
+      <c r="N24">
+        <v>100</v>
+      </c>
+      <c r="O24">
+        <v>75</v>
+      </c>
+      <c r="P24" s="10">
+        <v>0.17180000000000001</v>
+      </c>
+      <c r="Q24">
+        <v>119.62569999999999</v>
+      </c>
+      <c r="R24">
+        <v>168.05760000000001</v>
+      </c>
+      <c r="S24">
+        <v>128.7296</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F1:K1"/>
-    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added values for Finland
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="22">
   <si>
     <t>Belgium</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>adapt.size.start</t>
+  </si>
+  <si>
+    <t>Finland</t>
   </si>
 </sst>
 </file>
@@ -157,16 +160,87 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -442,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,19 +533,19 @@
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
@@ -483,11 +557,11 @@
       <c r="P1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
       <c r="T1" s="3" t="s">
         <v>11</v>
       </c>
@@ -503,18 +577,18 @@
       <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="10"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
@@ -1409,6 +1483,12 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
       <c r="C23">
         <v>-1.75</v>
       </c>
@@ -1507,7 +1587,7 @@
       <c r="O24">
         <v>75</v>
       </c>
-      <c r="P24" s="10">
+      <c r="P24" s="9">
         <v>0.17180000000000001</v>
       </c>
       <c r="Q24">
@@ -1518,6 +1598,365 @@
       </c>
       <c r="S24">
         <v>128.7296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>-1.5</v>
+      </c>
+      <c r="D27">
+        <v>-0.05</v>
+      </c>
+      <c r="E27">
+        <v>-0.25</v>
+      </c>
+      <c r="F27">
+        <v>-2.5</v>
+      </c>
+      <c r="G27">
+        <v>-1.5</v>
+      </c>
+      <c r="H27">
+        <v>-0.1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>-0.1</v>
+      </c>
+      <c r="K27">
+        <v>0.1</v>
+      </c>
+      <c r="L27">
+        <v>0.01</v>
+      </c>
+      <c r="M27">
+        <v>2000</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27">
+        <v>75</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0.1205</v>
+      </c>
+      <c r="Q27">
+        <v>20.574570000000001</v>
+      </c>
+      <c r="R27">
+        <v>53.038080000000001</v>
+      </c>
+      <c r="S27">
+        <v>19.133959999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>-2.25</v>
+      </c>
+      <c r="D28">
+        <v>-0.05</v>
+      </c>
+      <c r="E28">
+        <v>-0.25</v>
+      </c>
+      <c r="F28">
+        <v>-3.5</v>
+      </c>
+      <c r="G28">
+        <v>-1</v>
+      </c>
+      <c r="H28">
+        <v>-0.1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>-0.1</v>
+      </c>
+      <c r="K28">
+        <v>0.1</v>
+      </c>
+      <c r="L28">
+        <v>0.01</v>
+      </c>
+      <c r="M28">
+        <v>2000</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
+      <c r="O28">
+        <v>75</v>
+      </c>
+      <c r="P28" s="2">
+        <v>0.113</v>
+      </c>
+      <c r="Q28">
+        <v>38.494610000000002</v>
+      </c>
+      <c r="R28">
+        <v>60.992919999999998</v>
+      </c>
+      <c r="S28">
+        <v>58.892090000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>-2.75</v>
+      </c>
+      <c r="D29">
+        <v>-0.05</v>
+      </c>
+      <c r="E29">
+        <v>-0.05</v>
+      </c>
+      <c r="F29">
+        <v>-3.5</v>
+      </c>
+      <c r="G29">
+        <v>-2</v>
+      </c>
+      <c r="H29">
+        <v>-0.1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>-0.1</v>
+      </c>
+      <c r="K29">
+        <v>0.1</v>
+      </c>
+      <c r="L29">
+        <v>0.01</v>
+      </c>
+      <c r="M29">
+        <v>2000</v>
+      </c>
+      <c r="N29">
+        <v>100</v>
+      </c>
+      <c r="O29">
+        <v>75</v>
+      </c>
+      <c r="P29" s="2">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="Q29">
+        <v>33.39472</v>
+      </c>
+      <c r="R29">
+        <v>121.38133000000001</v>
+      </c>
+      <c r="S29">
+        <v>50.981999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>-2.75</v>
+      </c>
+      <c r="D30">
+        <v>-0.05</v>
+      </c>
+      <c r="E30">
+        <v>-0.05</v>
+      </c>
+      <c r="F30">
+        <v>-3</v>
+      </c>
+      <c r="G30">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H30">
+        <v>-0.05</v>
+      </c>
+      <c r="I30">
+        <v>0.05</v>
+      </c>
+      <c r="J30">
+        <v>-0.05</v>
+      </c>
+      <c r="K30">
+        <v>0.1</v>
+      </c>
+      <c r="L30">
+        <v>0.01</v>
+      </c>
+      <c r="M30">
+        <v>2000</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
+      </c>
+      <c r="O30">
+        <v>75</v>
+      </c>
+      <c r="P30" s="2">
+        <v>0.182</v>
+      </c>
+      <c r="Q30">
+        <v>95.302019999999999</v>
+      </c>
+      <c r="R30">
+        <v>94.160520000000005</v>
+      </c>
+      <c r="S30">
+        <v>84.330979999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>-2.75</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>-3</v>
+      </c>
+      <c r="G31">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H31">
+        <v>-0.05</v>
+      </c>
+      <c r="I31">
+        <v>0.05</v>
+      </c>
+      <c r="J31">
+        <v>-0.05</v>
+      </c>
+      <c r="K31">
+        <v>0.1</v>
+      </c>
+      <c r="L31">
+        <v>0.01</v>
+      </c>
+      <c r="M31">
+        <v>2000</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31">
+        <v>75</v>
+      </c>
+      <c r="P31" s="2">
+        <v>0.32750000000000001</v>
+      </c>
+      <c r="Q31">
+        <v>186.1704</v>
+      </c>
+      <c r="R31">
+        <v>194.44460000000001</v>
+      </c>
+      <c r="S31">
+        <v>198.20070000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>-2.75</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>-3</v>
+      </c>
+      <c r="G32">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H32">
+        <v>-0.05</v>
+      </c>
+      <c r="I32">
+        <v>0.05</v>
+      </c>
+      <c r="J32">
+        <v>-0.05</v>
+      </c>
+      <c r="K32">
+        <v>0.1</v>
+      </c>
+      <c r="L32">
+        <v>0.01</v>
+      </c>
+      <c r="M32">
+        <v>10000</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32">
+        <v>75</v>
+      </c>
+      <c r="P32" s="2">
+        <v>0.27450000000000002</v>
+      </c>
+      <c r="Q32">
+        <v>619.47239999999999</v>
+      </c>
+      <c r="R32">
+        <v>609.1472</v>
+      </c>
+      <c r="S32">
+        <v>631.30150000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1529,6 +1968,60 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F1:K1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E8:E30">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="notBetween">
+      <formula>$J$27</formula>
+      <formula>$K$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D30">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="notBetween">
+      <formula>$H$8</formula>
+      <formula>$I$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C30">
+    <cfRule type="cellIs" priority="7" operator="notBetween">
+      <formula>$F$8</formula>
+      <formula>$G$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="notBetween">
+      <formula>$J$27</formula>
+      <formula>$K$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="notBetween">
+      <formula>$H$8</formula>
+      <formula>$I$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="cellIs" priority="4" operator="notBetween">
+      <formula>$F$8</formula>
+      <formula>$G$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
+      <formula>$J$27</formula>
+      <formula>$K$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
+      <formula>$H$8</formula>
+      <formula>$I$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="cellIs" priority="1" operator="notBetween">
+      <formula>$F$8</formula>
+      <formula>$G$8</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added values for Germany and removed starting values outside of or on limit of prior range
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>Belgium</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Finland</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -516,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W29" sqref="W29"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,16 +778,16 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <v>-1.5</v>
+        <v>-1.75</v>
       </c>
       <c r="D8">
         <v>-0.05</v>
       </c>
       <c r="E8">
-        <v>-0.25</v>
+        <v>-0.05</v>
       </c>
       <c r="F8">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="G8">
         <v>-1</v>
@@ -786,10 +799,10 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L8">
         <v>0.01</v>
@@ -798,22 +811,22 @@
         <v>2000</v>
       </c>
       <c r="N8">
+        <v>200</v>
+      </c>
+      <c r="O8">
         <v>100</v>
       </c>
-      <c r="O8">
-        <v>75</v>
-      </c>
       <c r="P8" s="7">
-        <v>0.18099999999999999</v>
+        <v>0.19450000000000001</v>
       </c>
       <c r="Q8">
-        <v>66.404989999999998</v>
+        <v>42.790819999999997</v>
       </c>
       <c r="R8">
-        <v>62.142000000000003</v>
+        <v>57.035820000000001</v>
       </c>
       <c r="S8">
-        <v>56.486499999999999</v>
+        <v>54.978209999999997</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -824,19 +837,19 @@
         <v>16</v>
       </c>
       <c r="C9">
-        <v>-1.5</v>
+        <v>-1.75</v>
       </c>
       <c r="D9">
         <v>-0.05</v>
       </c>
       <c r="E9">
-        <v>-0.25</v>
+        <v>-0.05</v>
       </c>
       <c r="F9">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="G9">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="H9">
         <v>-0.1</v>
@@ -863,16 +876,16 @@
         <v>75</v>
       </c>
       <c r="P9" s="7">
-        <v>0.28000000000000003</v>
+        <v>0.219</v>
       </c>
       <c r="Q9">
-        <v>124.1626</v>
+        <v>60.325539999999997</v>
       </c>
       <c r="R9">
-        <v>128.38419999999999</v>
+        <v>60.738010000000003</v>
       </c>
       <c r="S9">
-        <v>139.61969999999999</v>
+        <v>60.348730000000003</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -883,19 +896,19 @@
         <v>16</v>
       </c>
       <c r="C10">
-        <v>-1.7</v>
+        <v>-1.75</v>
       </c>
       <c r="D10">
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="F10">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="G10">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="H10">
         <v>-0.1</v>
@@ -913,7 +926,7 @@
         <v>0.01</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="N10">
         <v>100</v>
@@ -921,167 +934,54 @@
       <c r="O10">
         <v>75</v>
       </c>
-      <c r="P10" s="7">
-        <v>0.30099999999999999</v>
+      <c r="P10" s="9">
+        <v>0.17180000000000001</v>
       </c>
       <c r="Q10">
-        <v>94.651880000000006</v>
+        <v>119.62569999999999</v>
       </c>
       <c r="R10">
-        <v>96.072630000000004</v>
+        <v>168.05760000000001</v>
       </c>
       <c r="S10">
-        <v>79.661850000000001</v>
+        <v>128.7296</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>-1.5</v>
-      </c>
-      <c r="D11">
-        <v>-0.05</v>
-      </c>
-      <c r="E11">
-        <v>-0.25</v>
-      </c>
-      <c r="F11">
-        <v>-2</v>
-      </c>
-      <c r="G11">
-        <v>-1.5</v>
-      </c>
-      <c r="H11">
-        <v>-0.1</v>
-      </c>
-      <c r="I11">
-        <v>0.1</v>
-      </c>
-      <c r="J11">
-        <v>-0.1</v>
-      </c>
-      <c r="K11">
-        <v>0.1</v>
-      </c>
-      <c r="L11">
-        <v>0.01</v>
-      </c>
       <c r="M11">
-        <v>2000</v>
-      </c>
-      <c r="N11">
-        <v>100</v>
-      </c>
-      <c r="O11">
-        <v>75</v>
-      </c>
-      <c r="P11" s="7">
-        <v>0.30199999999999999</v>
-      </c>
-      <c r="Q11">
-        <v>123.7658</v>
-      </c>
-      <c r="R11">
-        <v>146.19380000000001</v>
-      </c>
-      <c r="S11">
-        <v>132.3364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>-1.5</v>
-      </c>
-      <c r="D12">
-        <v>-0.05</v>
-      </c>
-      <c r="E12">
-        <v>-0.25</v>
-      </c>
-      <c r="F12">
-        <v>-1.9</v>
-      </c>
-      <c r="G12">
-        <v>-1.6</v>
-      </c>
-      <c r="H12">
-        <v>-0.1</v>
-      </c>
-      <c r="I12">
-        <v>0.1</v>
-      </c>
-      <c r="J12">
-        <v>-0.1</v>
-      </c>
-      <c r="K12">
-        <v>0.1</v>
-      </c>
-      <c r="L12">
-        <v>0.01</v>
-      </c>
-      <c r="M12">
-        <v>2000</v>
-      </c>
-      <c r="N12">
-        <v>100</v>
-      </c>
-      <c r="O12">
-        <v>75</v>
-      </c>
-      <c r="P12" s="7">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="Q12">
-        <v>122.751</v>
-      </c>
-      <c r="R12">
-        <v>151.02969999999999</v>
-      </c>
-      <c r="S12">
-        <v>115.8591</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13">
-        <v>-1.5</v>
+        <v>-2.75</v>
       </c>
       <c r="D13">
         <v>-0.05</v>
       </c>
       <c r="E13">
-        <v>-0.25</v>
+        <v>-0.05</v>
       </c>
       <c r="F13">
-        <v>-1.9</v>
+        <v>-3.5</v>
       </c>
       <c r="G13">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="H13">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K13">
         <v>0.1</v>
@@ -1098,49 +998,49 @@
       <c r="O13">
         <v>75</v>
       </c>
-      <c r="P13" s="7">
-        <v>0.33750000000000002</v>
+      <c r="P13" s="2">
+        <v>0.17899999999999999</v>
       </c>
       <c r="Q13">
-        <v>147.4735</v>
+        <v>33.39472</v>
       </c>
       <c r="R13">
-        <v>172.30279999999999</v>
+        <v>121.38133000000001</v>
       </c>
       <c r="S13">
-        <v>222.35339999999999</v>
+        <v>50.981999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14">
-        <v>-1.5</v>
+        <v>-2.75</v>
       </c>
       <c r="D14">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>-1.9</v>
+        <v>-3</v>
       </c>
       <c r="G14">
-        <v>-1.8</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="H14">
         <v>-0.05</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J14">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="K14">
         <v>0.1</v>
@@ -1157,58 +1057,58 @@
       <c r="O14">
         <v>75</v>
       </c>
-      <c r="P14" s="7">
-        <v>0.35949999999999999</v>
+      <c r="P14" s="2">
+        <v>0.32750000000000001</v>
       </c>
       <c r="Q14">
-        <v>205.1311</v>
+        <v>186.1704</v>
       </c>
       <c r="R14">
-        <v>204.77430000000001</v>
+        <v>194.44460000000001</v>
       </c>
       <c r="S14">
-        <v>212.88749999999999</v>
+        <v>198.20070000000001</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15">
-        <v>-1.5</v>
+        <v>-2.75</v>
       </c>
       <c r="D15">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>-1.9</v>
+        <v>-3</v>
       </c>
       <c r="G15">
-        <v>-1.8</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="H15">
         <v>-0.05</v>
       </c>
       <c r="I15">
+        <v>0.05</v>
+      </c>
+      <c r="J15">
+        <v>-0.05</v>
+      </c>
+      <c r="K15">
         <v>0.1</v>
-      </c>
-      <c r="J15">
-        <v>-0.1</v>
-      </c>
-      <c r="K15">
-        <v>0.05</v>
       </c>
       <c r="L15">
         <v>0.01</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N15">
         <v>100</v>
@@ -1216,100 +1116,52 @@
       <c r="O15">
         <v>75</v>
       </c>
-      <c r="P15" s="7">
-        <v>0.42599999999999999</v>
+      <c r="P15" s="2">
+        <v>0.27450000000000002</v>
       </c>
       <c r="Q15">
-        <v>150.15469999999999</v>
+        <v>619.47239999999999</v>
       </c>
       <c r="R15">
-        <v>245.08179999999999</v>
+        <v>609.1472</v>
       </c>
       <c r="S15">
-        <v>209.4426</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17">
-        <v>-1.5</v>
-      </c>
-      <c r="D17">
-        <v>-0.05</v>
-      </c>
-      <c r="E17">
-        <v>-0.25</v>
-      </c>
-      <c r="F17">
-        <v>-2.5</v>
-      </c>
-      <c r="G17">
-        <v>-0.5</v>
-      </c>
-      <c r="H17">
-        <v>-0.1</v>
-      </c>
-      <c r="I17">
-        <v>0.05</v>
-      </c>
-      <c r="J17">
-        <v>-0.2</v>
-      </c>
-      <c r="K17">
-        <v>0.2</v>
-      </c>
-      <c r="L17">
-        <v>0.01</v>
-      </c>
-      <c r="M17">
-        <v>2000</v>
-      </c>
-      <c r="N17">
-        <v>100</v>
-      </c>
-      <c r="O17">
-        <v>75</v>
-      </c>
-      <c r="P17" s="7"/>
+        <v>631.30150000000003</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>-2.5</v>
+        <v>-5</v>
       </c>
       <c r="G18">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H18">
         <v>-0.1</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J18">
-        <v>-0.15</v>
+        <v>-0.1</v>
       </c>
       <c r="K18">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="L18">
         <v>0.01</v>
@@ -1323,88 +1175,167 @@
       <c r="O18">
         <v>75</v>
       </c>
-      <c r="P18" s="7"/>
+      <c r="P18" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="Q18">
+        <v>26.320589999999999</v>
+      </c>
+      <c r="R18">
+        <v>39.075009999999999</v>
+      </c>
+      <c r="S18">
+        <v>31.292940000000002</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19">
-        <v>-1.5</v>
+        <v>-2.5</v>
       </c>
       <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.05</v>
+      </c>
+      <c r="F19">
+        <v>-3</v>
+      </c>
+      <c r="G19">
+        <v>-2</v>
+      </c>
+      <c r="H19">
         <v>-0.05</v>
       </c>
-      <c r="E19">
-        <v>-0.25</v>
-      </c>
-      <c r="F19">
-        <v>-2.5</v>
-      </c>
-      <c r="G19">
-        <v>-1</v>
-      </c>
-      <c r="H19">
-        <v>-0.1</v>
-      </c>
       <c r="I19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J19">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="L19">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="M19">
         <v>2000</v>
       </c>
       <c r="N19">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O19">
+        <v>75</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0.188</v>
+      </c>
+      <c r="Q19">
+        <v>80.213939999999994</v>
+      </c>
+      <c r="R19">
+        <v>87.504679999999993</v>
+      </c>
+      <c r="S19">
+        <v>84.241979999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>-2.8</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F20">
+        <v>-3</v>
+      </c>
+      <c r="G20">
+        <v>-2.6</v>
+      </c>
+      <c r="H20">
+        <v>-0.05</v>
+      </c>
+      <c r="I20">
+        <v>0.1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0.1</v>
+      </c>
+      <c r="L20">
+        <v>0.01</v>
+      </c>
+      <c r="M20">
+        <v>2000</v>
+      </c>
+      <c r="N20">
         <v>100</v>
       </c>
-      <c r="P19" s="7">
-        <v>0.13400000000000001</v>
+      <c r="O20">
+        <v>75</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0.23250000000000001</v>
+      </c>
+      <c r="Q20">
+        <v>112.68683</v>
+      </c>
+      <c r="R20">
+        <v>136.29983999999999</v>
+      </c>
+      <c r="S20">
+        <v>57.85284</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21">
-        <v>-1.5</v>
+        <v>-2.8</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F21">
+        <v>-3</v>
+      </c>
+      <c r="G21">
+        <v>-2.6</v>
+      </c>
+      <c r="H21">
         <v>-0.05</v>
       </c>
-      <c r="E21">
-        <v>-0.25</v>
-      </c>
-      <c r="F21">
-        <v>-2.5</v>
-      </c>
-      <c r="G21">
-        <v>-1.5</v>
-      </c>
-      <c r="H21">
-        <v>-0.1</v>
-      </c>
       <c r="I21">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J21">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0.1</v>
@@ -1413,550 +1344,25 @@
         <v>0.01</v>
       </c>
       <c r="M21">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N21">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O21">
-        <v>100</v>
-      </c>
-      <c r="P21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22">
-        <v>-1.75</v>
-      </c>
-      <c r="D22">
-        <v>-0.05</v>
-      </c>
-      <c r="E22">
-        <v>-0.05</v>
-      </c>
-      <c r="F22">
-        <v>-2.5</v>
-      </c>
-      <c r="G22">
-        <v>-1</v>
-      </c>
-      <c r="H22">
-        <v>-0.1</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>-0.1</v>
-      </c>
-      <c r="K22">
-        <v>0.1</v>
-      </c>
-      <c r="L22">
-        <v>0.01</v>
-      </c>
-      <c r="M22">
-        <v>2000</v>
-      </c>
-      <c r="N22">
-        <v>200</v>
-      </c>
-      <c r="O22">
-        <v>100</v>
-      </c>
-      <c r="P22" s="7">
-        <v>0.19450000000000001</v>
-      </c>
-      <c r="Q22">
-        <v>42.790819999999997</v>
-      </c>
-      <c r="R22">
-        <v>57.035820000000001</v>
-      </c>
-      <c r="S22">
-        <v>54.978209999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23">
-        <v>-1.75</v>
-      </c>
-      <c r="D23">
-        <v>-0.05</v>
-      </c>
-      <c r="E23">
-        <v>-0.05</v>
-      </c>
-      <c r="F23">
-        <v>-2.5</v>
-      </c>
-      <c r="G23">
-        <v>-1</v>
-      </c>
-      <c r="H23">
-        <v>-0.1</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>-0.1</v>
-      </c>
-      <c r="K23">
-        <v>0.1</v>
-      </c>
-      <c r="L23">
-        <v>0.01</v>
-      </c>
-      <c r="M23">
-        <v>2000</v>
-      </c>
-      <c r="N23">
-        <v>100</v>
-      </c>
-      <c r="O23">
         <v>75</v>
       </c>
-      <c r="P23" s="7">
-        <v>0.219</v>
-      </c>
-      <c r="Q23">
-        <v>60.325539999999997</v>
-      </c>
-      <c r="R23">
-        <v>60.738010000000003</v>
-      </c>
-      <c r="S23">
-        <v>60.348730000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24">
-        <v>-1.75</v>
-      </c>
-      <c r="D24">
-        <v>-0.05</v>
-      </c>
-      <c r="E24">
-        <v>-0.05</v>
-      </c>
-      <c r="F24">
-        <v>-2.5</v>
-      </c>
-      <c r="G24">
-        <v>-1</v>
-      </c>
-      <c r="H24">
-        <v>-0.1</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>-0.1</v>
-      </c>
-      <c r="K24">
-        <v>0.1</v>
-      </c>
-      <c r="L24">
-        <v>0.01</v>
-      </c>
-      <c r="M24">
-        <v>5000</v>
-      </c>
-      <c r="N24">
-        <v>100</v>
-      </c>
-      <c r="O24">
-        <v>75</v>
-      </c>
-      <c r="P24" s="9">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="Q24">
-        <v>119.62569999999999</v>
-      </c>
-      <c r="R24">
-        <v>168.05760000000001</v>
-      </c>
-      <c r="S24">
-        <v>128.7296</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M25">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27">
-        <v>-1.5</v>
-      </c>
-      <c r="D27">
-        <v>-0.05</v>
-      </c>
-      <c r="E27">
-        <v>-0.25</v>
-      </c>
-      <c r="F27">
-        <v>-2.5</v>
-      </c>
-      <c r="G27">
-        <v>-1.5</v>
-      </c>
-      <c r="H27">
-        <v>-0.1</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>-0.1</v>
-      </c>
-      <c r="K27">
-        <v>0.1</v>
-      </c>
-      <c r="L27">
-        <v>0.01</v>
-      </c>
-      <c r="M27">
-        <v>2000</v>
-      </c>
-      <c r="N27">
-        <v>100</v>
-      </c>
-      <c r="O27">
-        <v>75</v>
-      </c>
-      <c r="P27" s="2">
-        <v>0.1205</v>
-      </c>
-      <c r="Q27">
-        <v>20.574570000000001</v>
-      </c>
-      <c r="R27">
-        <v>53.038080000000001</v>
-      </c>
-      <c r="S27">
-        <v>19.133959999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28">
-        <v>-2.25</v>
-      </c>
-      <c r="D28">
-        <v>-0.05</v>
-      </c>
-      <c r="E28">
-        <v>-0.25</v>
-      </c>
-      <c r="F28">
-        <v>-3.5</v>
-      </c>
-      <c r="G28">
-        <v>-1</v>
-      </c>
-      <c r="H28">
-        <v>-0.1</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>-0.1</v>
-      </c>
-      <c r="K28">
-        <v>0.1</v>
-      </c>
-      <c r="L28">
-        <v>0.01</v>
-      </c>
-      <c r="M28">
-        <v>2000</v>
-      </c>
-      <c r="N28">
-        <v>100</v>
-      </c>
-      <c r="O28">
-        <v>75</v>
-      </c>
-      <c r="P28" s="2">
-        <v>0.113</v>
-      </c>
-      <c r="Q28">
-        <v>38.494610000000002</v>
-      </c>
-      <c r="R28">
-        <v>60.992919999999998</v>
-      </c>
-      <c r="S28">
-        <v>58.892090000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29">
-        <v>-2.75</v>
-      </c>
-      <c r="D29">
-        <v>-0.05</v>
-      </c>
-      <c r="E29">
-        <v>-0.05</v>
-      </c>
-      <c r="F29">
-        <v>-3.5</v>
-      </c>
-      <c r="G29">
-        <v>-2</v>
-      </c>
-      <c r="H29">
-        <v>-0.1</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>-0.1</v>
-      </c>
-      <c r="K29">
-        <v>0.1</v>
-      </c>
-      <c r="L29">
-        <v>0.01</v>
-      </c>
-      <c r="M29">
-        <v>2000</v>
-      </c>
-      <c r="N29">
-        <v>100</v>
-      </c>
-      <c r="O29">
-        <v>75</v>
-      </c>
-      <c r="P29" s="2">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="Q29">
-        <v>33.39472</v>
-      </c>
-      <c r="R29">
-        <v>121.38133000000001</v>
-      </c>
-      <c r="S29">
-        <v>50.981999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30">
-        <v>-2.75</v>
-      </c>
-      <c r="D30">
-        <v>-0.05</v>
-      </c>
-      <c r="E30">
-        <v>-0.05</v>
-      </c>
-      <c r="F30">
-        <v>-3</v>
-      </c>
-      <c r="G30">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="H30">
-        <v>-0.05</v>
-      </c>
-      <c r="I30">
-        <v>0.05</v>
-      </c>
-      <c r="J30">
-        <v>-0.05</v>
-      </c>
-      <c r="K30">
-        <v>0.1</v>
-      </c>
-      <c r="L30">
-        <v>0.01</v>
-      </c>
-      <c r="M30">
-        <v>2000</v>
-      </c>
-      <c r="N30">
-        <v>100</v>
-      </c>
-      <c r="O30">
-        <v>75</v>
-      </c>
-      <c r="P30" s="2">
-        <v>0.182</v>
-      </c>
-      <c r="Q30">
-        <v>95.302019999999999</v>
-      </c>
-      <c r="R30">
-        <v>94.160520000000005</v>
-      </c>
-      <c r="S30">
-        <v>84.330979999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31">
-        <v>-2.75</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>-3</v>
-      </c>
-      <c r="G31">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="H31">
-        <v>-0.05</v>
-      </c>
-      <c r="I31">
-        <v>0.05</v>
-      </c>
-      <c r="J31">
-        <v>-0.05</v>
-      </c>
-      <c r="K31">
-        <v>0.1</v>
-      </c>
-      <c r="L31">
-        <v>0.01</v>
-      </c>
-      <c r="M31">
-        <v>2000</v>
-      </c>
-      <c r="N31">
-        <v>100</v>
-      </c>
-      <c r="O31">
-        <v>75</v>
-      </c>
-      <c r="P31" s="2">
-        <v>0.32750000000000001</v>
-      </c>
-      <c r="Q31">
-        <v>186.1704</v>
-      </c>
-      <c r="R31">
-        <v>194.44460000000001</v>
-      </c>
-      <c r="S31">
-        <v>198.20070000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32">
-        <v>-2.75</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>-3</v>
-      </c>
-      <c r="G32">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="H32">
-        <v>-0.05</v>
-      </c>
-      <c r="I32">
-        <v>0.05</v>
-      </c>
-      <c r="J32">
-        <v>-0.05</v>
-      </c>
-      <c r="K32">
-        <v>0.1</v>
-      </c>
-      <c r="L32">
-        <v>0.01</v>
-      </c>
-      <c r="M32">
-        <v>10000</v>
-      </c>
-      <c r="N32">
-        <v>100</v>
-      </c>
-      <c r="O32">
-        <v>75</v>
-      </c>
-      <c r="P32" s="2">
-        <v>0.27450000000000002</v>
-      </c>
-      <c r="Q32">
-        <v>619.47239999999999</v>
-      </c>
-      <c r="R32">
-        <v>609.1472</v>
-      </c>
-      <c r="S32">
-        <v>631.30150000000003</v>
+      <c r="P21" s="2">
+        <v>0.2351</v>
+      </c>
+      <c r="Q21">
+        <v>478.86189999999999</v>
+      </c>
+      <c r="R21">
+        <v>619.19320000000005</v>
+      </c>
+      <c r="S21">
+        <v>514.95309999999995</v>
       </c>
     </row>
   </sheetData>
@@ -1968,58 +1374,76 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E8:E30">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="notBetween">
-      <formula>$J$27</formula>
-      <formula>$K$27</formula>
+  <conditionalFormatting sqref="E8:E14">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D30">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="notBetween">
-      <formula>$H$8</formula>
-      <formula>$I$8</formula>
+  <conditionalFormatting sqref="D8:D14">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C30">
-    <cfRule type="cellIs" priority="7" operator="notBetween">
-      <formula>$F$8</formula>
-      <formula>$G$8</formula>
+  <conditionalFormatting sqref="C8:C14">
+    <cfRule type="cellIs" priority="13" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="notBetween">
-      <formula>$J$27</formula>
-      <formula>$K$27</formula>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="notBetween">
-      <formula>$H$8</formula>
-      <formula>$I$8</formula>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" priority="4" operator="notBetween">
-      <formula>$F$8</formula>
-      <formula>$G$8</formula>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" priority="10" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
-      <formula>$J$27</formula>
-      <formula>$K$27</formula>
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
-      <formula>$H$8</formula>
-      <formula>$I$8</formula>
+  <conditionalFormatting sqref="D18:D20">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="cellIs" priority="4" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" priority="1" operator="notBetween">
-      <formula>$F$8</formula>
-      <formula>$G$8</formula>
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added updated values for Finland after using correct contact and mortality data as well as initial runs for a few additional countries
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>Belgium</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Germany</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>UK</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -529,16 +595,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
     <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -952,65 +1019,6 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>-2.75</v>
-      </c>
-      <c r="D13">
-        <v>-0.05</v>
-      </c>
-      <c r="E13">
-        <v>-0.05</v>
-      </c>
-      <c r="F13">
-        <v>-3.5</v>
-      </c>
-      <c r="G13">
-        <v>-2</v>
-      </c>
-      <c r="H13">
-        <v>-0.1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>-0.1</v>
-      </c>
-      <c r="K13">
-        <v>0.1</v>
-      </c>
-      <c r="L13">
-        <v>0.01</v>
-      </c>
-      <c r="M13">
-        <v>2000</v>
-      </c>
-      <c r="N13">
-        <v>100</v>
-      </c>
-      <c r="O13">
-        <v>75</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="Q13">
-        <v>33.39472</v>
-      </c>
-      <c r="R13">
-        <v>121.38133000000001</v>
-      </c>
-      <c r="S13">
-        <v>50.981999999999999</v>
-      </c>
-    </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
@@ -1022,25 +1030,25 @@
         <v>-2.75</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="F14">
-        <v>-3</v>
+        <v>-3.5</v>
       </c>
       <c r="G14">
-        <v>-2.2000000000000002</v>
+        <v>-2</v>
       </c>
       <c r="H14">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="I14">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="K14">
         <v>0.1</v>
@@ -1058,16 +1066,16 @@
         <v>75</v>
       </c>
       <c r="P14" s="2">
-        <v>0.32750000000000001</v>
+        <v>0.13150000000000001</v>
       </c>
       <c r="Q14">
-        <v>186.1704</v>
+        <v>60.392150000000001</v>
       </c>
       <c r="R14">
-        <v>194.44460000000001</v>
+        <v>70.976979999999998</v>
       </c>
       <c r="S14">
-        <v>198.20070000000001</v>
+        <v>32.176720000000003</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1108,7 +1116,7 @@
         <v>0.01</v>
       </c>
       <c r="M15">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N15">
         <v>100</v>
@@ -1117,135 +1125,124 @@
         <v>75</v>
       </c>
       <c r="P15" s="2">
-        <v>0.27450000000000002</v>
+        <v>0.1835</v>
       </c>
       <c r="Q15">
-        <v>619.47239999999999</v>
+        <v>65.100189999999998</v>
       </c>
       <c r="R15">
-        <v>609.1472</v>
+        <v>77.72542</v>
       </c>
       <c r="S15">
-        <v>631.30150000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
+        <v>93.688919999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>-5</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>-0.1</v>
-      </c>
-      <c r="I18">
-        <v>0.1</v>
-      </c>
-      <c r="J18">
-        <v>-0.1</v>
-      </c>
-      <c r="K18">
-        <v>0.1</v>
-      </c>
-      <c r="L18">
+      <c r="C16">
+        <v>-2.75</v>
+      </c>
+      <c r="D16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.05</v>
+      </c>
+      <c r="F16">
+        <v>-3</v>
+      </c>
+      <c r="G16">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0.05</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0.1</v>
+      </c>
+      <c r="L16">
         <v>0.01</v>
       </c>
-      <c r="M18">
+      <c r="M16">
         <v>2000</v>
       </c>
-      <c r="N18">
+      <c r="N16">
         <v>100</v>
       </c>
-      <c r="O18">
+      <c r="O16">
         <v>75</v>
       </c>
-      <c r="P18" s="2">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="Q18">
-        <v>26.320589999999999</v>
-      </c>
-      <c r="R18">
-        <v>39.075009999999999</v>
-      </c>
-      <c r="S18">
-        <v>31.292940000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="P16" s="2">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="Q16">
+        <v>94.709879999999998</v>
+      </c>
+      <c r="R16">
+        <v>82.742959999999997</v>
+      </c>
+      <c r="S16">
+        <v>148.25133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C19">
-        <v>-2.5</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
+      <c r="C17">
+        <v>-2.75</v>
+      </c>
+      <c r="D17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E17">
         <v>0.05</v>
       </c>
-      <c r="F19">
+      <c r="F17">
         <v>-3</v>
       </c>
-      <c r="G19">
-        <v>-2</v>
-      </c>
-      <c r="H19">
-        <v>-0.05</v>
-      </c>
-      <c r="I19">
-        <v>0.1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0.1</v>
-      </c>
-      <c r="L19">
+      <c r="G17">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0.05</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0.1</v>
+      </c>
+      <c r="L17">
         <v>0.01</v>
       </c>
-      <c r="M19">
-        <v>2000</v>
-      </c>
-      <c r="N19">
+      <c r="M17">
+        <v>10000</v>
+      </c>
+      <c r="N17">
         <v>100</v>
       </c>
-      <c r="O19">
+      <c r="O17">
         <v>75</v>
       </c>
-      <c r="P19" s="2">
-        <v>0.188</v>
-      </c>
-      <c r="Q19">
-        <v>80.213939999999994</v>
-      </c>
-      <c r="R19">
-        <v>87.504679999999993</v>
-      </c>
-      <c r="S19">
-        <v>84.241979999999998</v>
-      </c>
+      <c r="P17" s="2"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1255,28 +1252,28 @@
         <v>16</v>
       </c>
       <c r="C20">
-        <v>-2.8</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="G20">
-        <v>-2.6</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="I20">
         <v>0.1</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K20">
         <v>0.1</v>
@@ -1294,16 +1291,16 @@
         <v>75</v>
       </c>
       <c r="P20" s="2">
-        <v>0.23250000000000001</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="Q20">
-        <v>112.68683</v>
+        <v>26.320589999999999</v>
       </c>
       <c r="R20">
-        <v>136.29983999999999</v>
+        <v>39.075009999999999</v>
       </c>
       <c r="S20">
-        <v>57.85284</v>
+        <v>31.292940000000002</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -1314,19 +1311,19 @@
         <v>16</v>
       </c>
       <c r="C21">
-        <v>-2.8</v>
+        <v>-2.5</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F21">
         <v>-3</v>
       </c>
       <c r="G21">
-        <v>-2.6</v>
+        <v>-2</v>
       </c>
       <c r="H21">
         <v>-0.05</v>
@@ -1344,7 +1341,7 @@
         <v>0.01</v>
       </c>
       <c r="M21">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N21">
         <v>100</v>
@@ -1353,16 +1350,387 @@
         <v>75</v>
       </c>
       <c r="P21" s="2">
+        <v>0.188</v>
+      </c>
+      <c r="Q21">
+        <v>80.213939999999994</v>
+      </c>
+      <c r="R21">
+        <v>87.504679999999993</v>
+      </c>
+      <c r="S21">
+        <v>84.241979999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>-2.8</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F22">
+        <v>-3</v>
+      </c>
+      <c r="G22">
+        <v>-2.6</v>
+      </c>
+      <c r="H22">
+        <v>-0.05</v>
+      </c>
+      <c r="I22">
+        <v>0.1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0.1</v>
+      </c>
+      <c r="L22">
+        <v>0.01</v>
+      </c>
+      <c r="M22">
+        <v>2000</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
+      </c>
+      <c r="O22">
+        <v>75</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0.23250000000000001</v>
+      </c>
+      <c r="Q22">
+        <v>112.68683</v>
+      </c>
+      <c r="R22">
+        <v>136.29983999999999</v>
+      </c>
+      <c r="S22">
+        <v>57.85284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>-2.8</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F23">
+        <v>-3</v>
+      </c>
+      <c r="G23">
+        <v>-2.6</v>
+      </c>
+      <c r="H23">
+        <v>-0.05</v>
+      </c>
+      <c r="I23">
+        <v>0.1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0.1</v>
+      </c>
+      <c r="L23">
+        <v>0.01</v>
+      </c>
+      <c r="M23">
+        <v>10000</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23">
+        <v>75</v>
+      </c>
+      <c r="P23" s="2">
         <v>0.2351</v>
       </c>
-      <c r="Q21">
+      <c r="Q23">
         <v>478.86189999999999</v>
       </c>
-      <c r="R21">
+      <c r="R23">
         <v>619.19320000000005</v>
       </c>
-      <c r="S21">
+      <c r="S23">
         <v>514.95309999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>-5</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>-0.1</v>
+      </c>
+      <c r="I26">
+        <v>0.1</v>
+      </c>
+      <c r="J26">
+        <v>-0.1</v>
+      </c>
+      <c r="K26">
+        <v>0.1</v>
+      </c>
+      <c r="L26">
+        <v>0.01</v>
+      </c>
+      <c r="M26">
+        <v>2000</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
+      <c r="O26">
+        <v>75</v>
+      </c>
+      <c r="P26" s="2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="Q26">
+        <v>14.900119999999999</v>
+      </c>
+      <c r="R26">
+        <v>35.138979999999997</v>
+      </c>
+      <c r="S26">
+        <v>16.423549999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>-3.5</v>
+      </c>
+      <c r="D27">
+        <v>0.25</v>
+      </c>
+      <c r="E27">
+        <v>-0.25</v>
+      </c>
+      <c r="F27">
+        <v>-5</v>
+      </c>
+      <c r="G27">
+        <v>-2</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.5</v>
+      </c>
+      <c r="J27">
+        <v>-0.5</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0.01</v>
+      </c>
+      <c r="M27">
+        <v>2000</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27">
+        <v>75</v>
+      </c>
+      <c r="P27" s="2">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="Q27">
+        <v>14.234690000000001</v>
+      </c>
+      <c r="R27">
+        <v>29.072649999999999</v>
+      </c>
+      <c r="S27">
+        <v>22.865079999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>-7</v>
+      </c>
+      <c r="G28">
+        <v>-3.5</v>
+      </c>
+      <c r="H28">
+        <v>-0.5</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0.5</v>
+      </c>
+      <c r="L28">
+        <v>0.01</v>
+      </c>
+      <c r="M28">
+        <v>2000</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
+      <c r="O28">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>-5</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>-0.1</v>
+      </c>
+      <c r="I31">
+        <v>0.1</v>
+      </c>
+      <c r="J31">
+        <v>-0.1</v>
+      </c>
+      <c r="K31">
+        <v>0.1</v>
+      </c>
+      <c r="L31">
+        <v>0.01</v>
+      </c>
+      <c r="M31">
+        <v>2000</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31">
+        <v>75</v>
+      </c>
+      <c r="P31" s="2">
+        <v>5.0500000000000003E-2</v>
+      </c>
+      <c r="Q31">
+        <v>3.9583469999999998</v>
+      </c>
+      <c r="R31">
+        <v>3.5701999999999998</v>
+      </c>
+      <c r="S31">
+        <v>2.862905</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>-4</v>
+      </c>
+      <c r="G32">
+        <v>-1</v>
+      </c>
+      <c r="H32">
+        <v>-0.3</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0.1</v>
+      </c>
+      <c r="K32">
+        <v>0.5</v>
+      </c>
+      <c r="L32">
+        <v>0.01</v>
+      </c>
+      <c r="M32">
+        <v>2000</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1374,73 +1742,109 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E8:E14">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="notBetween">
+  <conditionalFormatting sqref="E8:E15">
+    <cfRule type="cellIs" dxfId="13" priority="24" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D14">
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="notBetween">
+  <conditionalFormatting sqref="D8:D15">
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C14">
-    <cfRule type="cellIs" priority="13" operator="notBetween">
+  <conditionalFormatting sqref="C8:C15">
+    <cfRule type="cellIs" priority="22" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="notBetween">
+  <conditionalFormatting sqref="E20:E22">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="notBetween">
+  <conditionalFormatting sqref="D20:D22">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" priority="10" operator="notBetween">
+  <conditionalFormatting sqref="C20:C22">
+    <cfRule type="cellIs" priority="13" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E20">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="notBetween">
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D20">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="notBetween">
+  <conditionalFormatting sqref="D23">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C20">
-    <cfRule type="cellIs" priority="4" operator="notBetween">
+  <conditionalFormatting sqref="C23">
+    <cfRule type="cellIs" priority="10" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
+  <conditionalFormatting sqref="E16:E17">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
+  <conditionalFormatting sqref="D16:D17">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C16:C17">
+    <cfRule type="cellIs" priority="7" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E28">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D28">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C28">
+    <cfRule type="cellIs" priority="4" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
+      <formula>#REF!</formula>
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
     <cfRule type="cellIs" priority="1" operator="notBetween">
       <formula>#REF!</formula>
       <formula>#REF!</formula>

</xml_diff>

<commit_message>
Updated with values for all 10K runs
</commit_message>
<xml_diff>
--- a/R/MCMC settings.xlsx
+++ b/R/MCMC settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="35">
   <si>
     <t>Belgium</t>
   </si>
@@ -127,6 +127,9 @@
   <si>
     <t>avg for 10000</t>
   </si>
+  <si>
+    <t>453.8998 342.9841</t>
+  </si>
 </sst>
 </file>
 
@@ -180,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,13 +202,16 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA80"/>
+  <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,19 +524,19 @@
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
       <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
@@ -542,11 +548,11 @@
       <c r="P1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
       <c r="T1" s="3" t="s">
         <v>11</v>
       </c>
@@ -571,18 +577,18 @@
       <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
@@ -786,7 +792,7 @@
       <c r="X6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" s="14" t="s">
+      <c r="AA6" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -800,14 +806,14 @@
       <c r="O7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="V7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
       <c r="AA7" s="8">
-        <f>AVERAGE(AA8:AA80)</f>
-        <v>0.22046249999999995</v>
+        <f>AVERAGE(AA8:AA1052)</f>
+        <v>0.21017272727272723</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -2738,15 +2744,15 @@
         <v>431</v>
       </c>
       <c r="V39" t="b">
-        <f t="shared" ref="V39:V67" si="7">IF(C39="","",IF(C39&gt;F39, IF(C39&lt;G39, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="V39:V73" si="7">IF(C39="","",IF(C39&gt;F39, IF(C39&lt;G39, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="W39" t="b">
-        <f t="shared" ref="W39:W67" si="8">IF(D39="","",IF(D39&gt;H39, IF(D39&lt;I39, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="W39:W73" si="8">IF(D39="","",IF(D39&gt;H39, IF(D39&lt;I39, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="X39" t="b">
-        <f t="shared" ref="X39:X67" si="9">IF(E39="","",IF(E39&gt;J39, IF(E39&lt;K39, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="X39:X73" si="9">IF(E39="","",IF(E39&gt;J39, IF(E39&lt;K39, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="AA39">
@@ -3622,6 +3628,33 @@
       <c r="B56" t="s">
         <v>16</v>
       </c>
+      <c r="C56">
+        <v>-4</v>
+      </c>
+      <c r="D56">
+        <v>-0.125</v>
+      </c>
+      <c r="E56">
+        <v>0.1</v>
+      </c>
+      <c r="F56">
+        <v>-5</v>
+      </c>
+      <c r="G56">
+        <v>-2.5</v>
+      </c>
+      <c r="H56">
+        <v>-0.25</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>-0.2</v>
+      </c>
+      <c r="K56">
+        <v>0.3</v>
+      </c>
       <c r="L56">
         <v>0.01</v>
       </c>
@@ -3634,18 +3667,29 @@
       <c r="O56">
         <v>75</v>
       </c>
-      <c r="P56" s="2"/>
-      <c r="V56" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="W56" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="X56" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="P56" s="2">
+        <v>0.17050000000000001</v>
+      </c>
+      <c r="Q56" s="13">
+        <v>40.426580000000001</v>
+      </c>
+      <c r="R56">
+        <v>54.662689999999998</v>
+      </c>
+      <c r="S56">
+        <v>43.768189999999997</v>
+      </c>
+      <c r="V56" t="b">
+        <f t="shared" ref="V56:V58" si="10">IF(C56="","",IF(C56&gt;F56, IF(C56&lt;G56, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="W56" t="b">
+        <f t="shared" ref="W56:W58" si="11">IF(D56="","",IF(D56&gt;H56, IF(D56&lt;I56, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X56" t="b">
+        <f t="shared" ref="X56:X58" si="12">IF(E56="","",IF(E56&gt;J56, IF(E56&lt;K56, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
       </c>
       <c r="AA56" t="str">
         <f t="shared" si="3"/>
@@ -3653,18 +3697,74 @@
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P57" s="2"/>
-      <c r="V57" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="W57" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="X57" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57">
+        <v>-4</v>
+      </c>
+      <c r="D57">
+        <v>-0.125</v>
+      </c>
+      <c r="E57">
+        <v>0.1</v>
+      </c>
+      <c r="F57">
+        <v>-5.5</v>
+      </c>
+      <c r="G57">
+        <v>-2.5</v>
+      </c>
+      <c r="H57">
+        <v>-0.25</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>-0.3</v>
+      </c>
+      <c r="K57">
+        <v>0.5</v>
+      </c>
+      <c r="L57">
+        <v>0.01</v>
+      </c>
+      <c r="M57">
+        <v>2000</v>
+      </c>
+      <c r="N57">
+        <v>100</v>
+      </c>
+      <c r="O57">
+        <v>75</v>
+      </c>
+      <c r="P57" s="2">
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="Q57" s="13">
+        <v>35.811369999999997</v>
+      </c>
+      <c r="R57">
+        <v>72.53528</v>
+      </c>
+      <c r="S57">
+        <v>34.272939999999998</v>
+      </c>
+      <c r="V57" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="W57" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="X57" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="AA57" t="str">
         <f t="shared" si="3"/>
@@ -3672,18 +3772,74 @@
       </c>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="P58" s="2"/>
-      <c r="V58" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="W58" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="X58" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58">
+        <v>-4</v>
+      </c>
+      <c r="D58">
+        <v>-0.125</v>
+      </c>
+      <c r="E58">
+        <v>0.1</v>
+      </c>
+      <c r="F58">
+        <v>-6</v>
+      </c>
+      <c r="G58">
+        <v>-2.5</v>
+      </c>
+      <c r="H58">
+        <v>-0.25</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>-0.1</v>
+      </c>
+      <c r="K58">
+        <v>0.3</v>
+      </c>
+      <c r="L58">
+        <v>0.01</v>
+      </c>
+      <c r="M58">
+        <v>2000</v>
+      </c>
+      <c r="N58">
+        <v>100</v>
+      </c>
+      <c r="O58">
+        <v>75</v>
+      </c>
+      <c r="P58" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="Q58" s="13">
+        <v>14.28309</v>
+      </c>
+      <c r="R58">
+        <v>28.456309999999998</v>
+      </c>
+      <c r="S58">
+        <v>16.01699</v>
+      </c>
+      <c r="V58" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="W58" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="X58" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="AA58" t="str">
         <f t="shared" si="3"/>
@@ -3692,37 +3848,37 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
         <v>16</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F59">
         <v>-5</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="H59">
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="I59">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J59">
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="K59">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="L59">
         <v>0.01</v>
@@ -3736,28 +3892,28 @@
       <c r="O59">
         <v>75</v>
       </c>
-      <c r="P59" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="Q59">
-        <v>6.2671729999999997</v>
+      <c r="P59" s="2">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="Q59" s="13">
+        <v>61.70055</v>
       </c>
       <c r="R59">
-        <v>57.938744</v>
+        <v>90.399749999999997</v>
       </c>
       <c r="S59">
-        <v>2.946879</v>
+        <v>64.400989999999993</v>
       </c>
       <c r="V59" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="V59:V60" si="13">IF(C59="","",IF(C59&gt;F59, IF(C59&lt;G59, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="W59" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="W59:W60" si="14">IF(D59="","",IF(D59&gt;H59, IF(D59&lt;I59, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="X59" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="X59:X60" si="15">IF(E59="","",IF(E59&gt;J59, IF(E59&lt;K59, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="AA59" t="str">
@@ -3767,43 +3923,43 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B60" t="s">
         <v>16</v>
       </c>
       <c r="C60">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="D60">
-        <v>-0.1</v>
+        <v>-0.125</v>
       </c>
       <c r="E60">
-        <v>-1</v>
+        <v>0.1</v>
       </c>
       <c r="F60">
         <v>-5</v>
       </c>
       <c r="G60">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="H60">
         <v>-0.3</v>
       </c>
       <c r="I60">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>-2</v>
+        <v>-0.3</v>
       </c>
       <c r="K60">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="L60">
         <v>0.01</v>
       </c>
       <c r="M60">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N60">
         <v>100</v>
@@ -3812,178 +3968,63 @@
         <v>75</v>
       </c>
       <c r="P60" s="2">
-        <v>4.7E-2</v>
-      </c>
-      <c r="Q60">
-        <v>2.3134109999999999</v>
-      </c>
-      <c r="R60">
-        <v>3.7881070000000001</v>
-      </c>
-      <c r="S60">
-        <v>3.381033</v>
+        <v>0.19</v>
+      </c>
+      <c r="Q60" s="13">
+        <v>254.87629999999999</v>
+      </c>
+      <c r="R60" t="s">
+        <v>34</v>
       </c>
       <c r="V60" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="W60" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="X60" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="3"/>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P61" s="2"/>
+      <c r="V61" t="str">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="W60" t="b">
+        <v/>
+      </c>
+      <c r="W61" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="X60" t="b">
+        <v/>
+      </c>
+      <c r="X61" t="str">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AA60" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61">
-        <v>-5</v>
-      </c>
-      <c r="D61">
-        <v>0.05</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>-7</v>
-      </c>
-      <c r="G61">
-        <v>-3</v>
-      </c>
-      <c r="H61">
-        <v>-0.05</v>
-      </c>
-      <c r="I61">
-        <v>0.1</v>
-      </c>
-      <c r="J61">
-        <v>-0.4</v>
-      </c>
-      <c r="K61">
-        <v>0.4</v>
-      </c>
-      <c r="L61">
-        <v>0.01</v>
-      </c>
-      <c r="M61">
-        <v>2000</v>
-      </c>
-      <c r="N61">
-        <v>100</v>
-      </c>
-      <c r="O61">
-        <v>75</v>
-      </c>
-      <c r="P61" s="2">
-        <v>0.19450000000000001</v>
-      </c>
-      <c r="Q61">
-        <v>79.786619999999999</v>
-      </c>
-      <c r="R61">
-        <v>75.661749999999998</v>
-      </c>
-      <c r="S61">
-        <v>68.689490000000006</v>
-      </c>
-      <c r="V61" t="b">
+        <v/>
+      </c>
+      <c r="AA61" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P62" s="2"/>
+      <c r="V62" t="str">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="W61" t="b">
+        <v/>
+      </c>
+      <c r="W62" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="X61" t="b">
+        <v/>
+      </c>
+      <c r="X62" t="str">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AA61" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62">
-        <v>-6</v>
-      </c>
-      <c r="D62">
-        <v>-0.05</v>
-      </c>
-      <c r="E62">
-        <v>0.1</v>
-      </c>
-      <c r="F62">
-        <v>-7</v>
-      </c>
-      <c r="G62">
-        <v>-5</v>
-      </c>
-      <c r="H62">
-        <v>-0.1</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <v>0.2</v>
-      </c>
-      <c r="L62">
-        <v>0.01</v>
-      </c>
-      <c r="M62">
-        <v>2000</v>
-      </c>
-      <c r="N62">
-        <v>100</v>
-      </c>
-      <c r="O62">
-        <v>75</v>
-      </c>
-      <c r="P62" s="2">
-        <v>7.5499999999999998E-2</v>
-      </c>
-      <c r="Q62">
-        <v>7.6524570000000001</v>
-      </c>
-      <c r="R62">
-        <v>7.936032</v>
-      </c>
-      <c r="S62">
-        <v>7.4568240000000001</v>
-      </c>
-      <c r="V62" t="b">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="W62" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="X62" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AA62" t="str">
         <f t="shared" si="3"/>
@@ -3997,6 +4038,33 @@
       <c r="B63" t="s">
         <v>16</v>
       </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>-5</v>
+      </c>
+      <c r="G63">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>-0.1</v>
+      </c>
+      <c r="I63">
+        <v>0.1</v>
+      </c>
+      <c r="J63">
+        <v>-0.1</v>
+      </c>
+      <c r="K63">
+        <v>0.1</v>
+      </c>
       <c r="L63">
         <v>0.01</v>
       </c>
@@ -4009,17 +4077,29 @@
       <c r="O63">
         <v>75</v>
       </c>
-      <c r="V63" t="str">
+      <c r="P63" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="Q63">
+        <v>6.2671729999999997</v>
+      </c>
+      <c r="R63">
+        <v>57.938744</v>
+      </c>
+      <c r="S63">
+        <v>2.946879</v>
+      </c>
+      <c r="V63" t="b">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="W63" t="str">
+        <v>1</v>
+      </c>
+      <c r="W63" t="b">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="X63" t="str">
+        <v>1</v>
+      </c>
+      <c r="X63" t="b">
         <f t="shared" si="9"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA63" t="str">
         <f t="shared" si="3"/>
@@ -4027,17 +4107,74 @@
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V64" t="str">
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64">
+        <v>-3</v>
+      </c>
+      <c r="D64">
+        <v>-0.1</v>
+      </c>
+      <c r="E64">
+        <v>-1</v>
+      </c>
+      <c r="F64">
+        <v>-5</v>
+      </c>
+      <c r="G64">
+        <v>-1</v>
+      </c>
+      <c r="H64">
+        <v>-0.3</v>
+      </c>
+      <c r="I64">
+        <v>0.1</v>
+      </c>
+      <c r="J64">
+        <v>-2</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0.01</v>
+      </c>
+      <c r="M64">
+        <v>2000</v>
+      </c>
+      <c r="N64">
+        <v>100</v>
+      </c>
+      <c r="O64">
+        <v>75</v>
+      </c>
+      <c r="P64" s="2">
+        <v>4.7E-2</v>
+      </c>
+      <c r="Q64">
+        <v>2.3134109999999999</v>
+      </c>
+      <c r="R64">
+        <v>3.7881070000000001</v>
+      </c>
+      <c r="S64">
+        <v>3.381033</v>
+      </c>
+      <c r="V64" t="b">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="W64" t="str">
+        <v>1</v>
+      </c>
+      <c r="W64" t="b">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="X64" t="str">
+        <v>1</v>
+      </c>
+      <c r="X64" t="b">
         <f t="shared" si="9"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA64" t="str">
         <f t="shared" si="3"/>
@@ -4045,17 +4182,74 @@
       </c>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V65" t="str">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65">
+        <v>-5</v>
+      </c>
+      <c r="D65">
+        <v>0.05</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>-7</v>
+      </c>
+      <c r="G65">
+        <v>-3</v>
+      </c>
+      <c r="H65">
+        <v>-0.05</v>
+      </c>
+      <c r="I65">
+        <v>0.1</v>
+      </c>
+      <c r="J65">
+        <v>-0.4</v>
+      </c>
+      <c r="K65">
+        <v>0.4</v>
+      </c>
+      <c r="L65">
+        <v>0.01</v>
+      </c>
+      <c r="M65">
+        <v>2000</v>
+      </c>
+      <c r="N65">
+        <v>100</v>
+      </c>
+      <c r="O65">
+        <v>75</v>
+      </c>
+      <c r="P65" s="2">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="Q65">
+        <v>79.786619999999999</v>
+      </c>
+      <c r="R65">
+        <v>75.661749999999998</v>
+      </c>
+      <c r="S65">
+        <v>68.689490000000006</v>
+      </c>
+      <c r="V65" t="b">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="W65" t="str">
+        <v>1</v>
+      </c>
+      <c r="W65" t="b">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="X65" t="str">
+        <v>1</v>
+      </c>
+      <c r="X65" t="b">
         <f t="shared" si="9"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AA65" t="str">
         <f t="shared" si="3"/>
@@ -4064,37 +4258,37 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
         <v>16</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F66">
+        <v>-7</v>
+      </c>
+      <c r="G66">
         <v>-5</v>
-      </c>
-      <c r="G66">
-        <v>5</v>
       </c>
       <c r="H66">
         <v>-0.1</v>
       </c>
       <c r="I66">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="K66">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="L66">
         <v>0.01</v>
@@ -4109,16 +4303,16 @@
         <v>75</v>
       </c>
       <c r="P66" s="2">
-        <v>5.0500000000000003E-2</v>
+        <v>7.5499999999999998E-2</v>
       </c>
       <c r="Q66">
-        <v>3.9583469999999998</v>
+        <v>7.6524570000000001</v>
       </c>
       <c r="R66">
-        <v>3.5701999999999998</v>
+        <v>7.936032</v>
       </c>
       <c r="S66">
-        <v>2.862905</v>
+        <v>7.4568240000000001</v>
       </c>
       <c r="V66" t="b">
         <f t="shared" si="7"/>
@@ -4139,34 +4333,34 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
         <v>16</v>
       </c>
       <c r="C67">
-        <v>-2.5</v>
+        <v>-5.5</v>
       </c>
       <c r="D67">
-        <v>-0.15</v>
+        <v>-0.05</v>
       </c>
       <c r="E67">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="F67">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="G67">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="H67">
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="I67">
         <v>0</v>
       </c>
       <c r="J67">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="K67">
         <v>0.5</v>
@@ -4184,16 +4378,16 @@
         <v>75</v>
       </c>
       <c r="P67" s="2">
-        <v>0.108</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="Q67">
-        <v>8.5242690000000003</v>
+        <v>35.700049999999997</v>
       </c>
       <c r="R67">
-        <v>12.167657</v>
+        <v>46.079929999999997</v>
       </c>
       <c r="S67">
-        <v>8.2206430000000008</v>
+        <v>88.602699999999999</v>
       </c>
       <c r="V67" t="b">
         <f t="shared" si="7"/>
@@ -4214,37 +4408,37 @@
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
         <v>16</v>
       </c>
       <c r="C68">
-        <v>-3.5</v>
+        <v>-5.75</v>
       </c>
       <c r="D68">
-        <v>-0.15</v>
+        <v>-0.05</v>
       </c>
       <c r="E68">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F68">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="G68">
-        <v>-2</v>
+        <v>-5.5</v>
       </c>
       <c r="H68">
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="I68">
         <v>0</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="K68">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="L68">
         <v>0.01</v>
@@ -4258,28 +4452,28 @@
       <c r="O68">
         <v>75</v>
       </c>
-      <c r="P68" s="11">
-        <v>8.6999999999999994E-2</v>
+      <c r="P68" s="2">
+        <v>0.26550000000000001</v>
       </c>
       <c r="Q68">
-        <v>3.6942210000000002</v>
+        <v>102.37482</v>
       </c>
       <c r="R68">
-        <v>5.7041209999999998</v>
+        <v>117.46015</v>
       </c>
       <c r="S68">
-        <v>4.7920980000000002</v>
+        <v>101.17709000000001</v>
       </c>
       <c r="V68" t="b">
-        <f t="shared" ref="V68" si="10">IF(C68="","",IF(C68&gt;F68, IF(C68&lt;G68, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="V68" si="16">IF(C68="","",IF(C68&gt;F68, IF(C68&lt;G68, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="W68" t="b">
-        <f t="shared" ref="W68" si="11">IF(D68="","",IF(D68&gt;H68, IF(D68&lt;I68, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="W68" si="17">IF(D68="","",IF(D68&gt;H68, IF(D68&lt;I68, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="X68" t="b">
-        <f t="shared" ref="X68" si="12">IF(E68="","",IF(E68&gt;J68, IF(E68&lt;K68, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="X68" si="18">IF(E68="","",IF(E68&gt;J68, IF(E68&lt;K68, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="AA68" t="str">
@@ -4289,43 +4483,43 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
         <v>16</v>
       </c>
       <c r="C69">
-        <v>-3.5</v>
+        <v>-5.75</v>
       </c>
       <c r="D69">
-        <v>-0.15</v>
+        <v>-0.05</v>
       </c>
       <c r="E69">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F69">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="G69">
-        <v>-2</v>
+        <v>-5.5</v>
       </c>
       <c r="H69">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="K69">
-        <v>2</v>
+        <v>0.15</v>
       </c>
       <c r="L69">
         <v>0.01</v>
       </c>
       <c r="M69">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N69">
         <v>100</v>
@@ -4333,104 +4527,47 @@
       <c r="O69">
         <v>75</v>
       </c>
-      <c r="P69" s="11">
-        <v>7.6499999999999999E-2</v>
+      <c r="P69" s="2">
+        <v>0.2145</v>
       </c>
       <c r="Q69">
-        <v>2.0420980000000002</v>
+        <v>7.0524019999999998</v>
       </c>
       <c r="R69">
-        <v>8.7851730000000003</v>
+        <v>39.970447</v>
       </c>
       <c r="S69">
-        <v>4.8587400000000001</v>
+        <v>24.409846000000002</v>
       </c>
       <c r="V69" t="b">
-        <f t="shared" ref="V69:V75" si="13">IF(C69="","",IF(C69&gt;F69, IF(C69&lt;G69, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="V69" si="19">IF(C69="","",IF(C69&gt;F69, IF(C69&lt;G69, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="W69" t="b">
-        <f t="shared" ref="W69:W75" si="14">IF(D69="","",IF(D69&gt;H69, IF(D69&lt;I69, TRUE, FALSE), FALSE))</f>
+        <f t="shared" ref="W69" si="20">IF(D69="","",IF(D69&gt;H69, IF(D69&lt;I69, TRUE, FALSE), FALSE))</f>
         <v>1</v>
       </c>
       <c r="X69" t="b">
-        <f t="shared" ref="X69:X75" si="15">IF(E69="","",IF(E69&gt;J69, IF(E69&lt;K69, TRUE, FALSE), FALSE))</f>
-        <v>1</v>
-      </c>
-      <c r="AA69" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" ref="X69" si="21">IF(E69="","",IF(E69&gt;J69, IF(E69&lt;K69, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA69">
+        <f t="shared" si="3"/>
+        <v>0.2145</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70">
-        <v>-5.5</v>
-      </c>
-      <c r="D70">
-        <v>-0.15</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>-9</v>
-      </c>
-      <c r="G70">
-        <v>-2</v>
-      </c>
-      <c r="H70">
-        <v>-0.5</v>
-      </c>
-      <c r="I70">
-        <v>0.5</v>
-      </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <v>2</v>
-      </c>
-      <c r="L70">
-        <v>0.01</v>
-      </c>
-      <c r="M70">
-        <v>2000</v>
-      </c>
-      <c r="N70">
-        <v>100</v>
-      </c>
-      <c r="O70">
-        <v>75</v>
-      </c>
-      <c r="P70" s="11">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="Q70">
-        <v>30.73854</v>
-      </c>
-      <c r="R70">
-        <v>47.048760000000001</v>
-      </c>
-      <c r="S70">
-        <v>19.026399999999999</v>
-      </c>
-      <c r="V70" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="W70" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="X70" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
+      <c r="V70" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="W70" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="X70" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
       <c r="AA70" t="str">
         <f t="shared" si="3"/>
@@ -4438,74 +4575,17 @@
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B71" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71">
-        <v>-5</v>
-      </c>
-      <c r="D71">
-        <v>-0.15</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71">
-        <v>-6</v>
-      </c>
-      <c r="G71">
-        <v>-4</v>
-      </c>
-      <c r="H71">
-        <v>-0.5</v>
-      </c>
-      <c r="I71">
-        <v>-0.05</v>
-      </c>
-      <c r="J71">
-        <v>0.5</v>
-      </c>
-      <c r="K71">
-        <v>2</v>
-      </c>
-      <c r="L71">
-        <v>0.01</v>
-      </c>
-      <c r="M71">
-        <v>2000</v>
-      </c>
-      <c r="N71">
-        <v>100</v>
-      </c>
-      <c r="O71">
-        <v>75</v>
-      </c>
-      <c r="P71" s="11">
-        <v>0.13450000000000001</v>
-      </c>
-      <c r="Q71">
-        <v>8.1231609999999996</v>
-      </c>
-      <c r="R71">
-        <v>27.910938999999999</v>
-      </c>
-      <c r="S71">
-        <v>16.052879000000001</v>
-      </c>
-      <c r="V71" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="W71" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="X71" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
+      <c r="V71" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="W71" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="X71" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
       <c r="AA71" t="str">
         <f t="shared" si="3"/>
@@ -4520,31 +4600,31 @@
         <v>16</v>
       </c>
       <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
         <v>-5</v>
       </c>
-      <c r="D72">
-        <v>-0.15</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72">
-        <v>-8</v>
-      </c>
       <c r="G72">
-        <v>-4</v>
+        <v>5</v>
       </c>
       <c r="H72">
-        <v>-0.25</v>
+        <v>-0.1</v>
       </c>
       <c r="I72">
-        <v>-0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J72">
-        <v>0.75</v>
+        <v>-0.1</v>
       </c>
       <c r="K72">
-        <v>1.25</v>
+        <v>0.1</v>
       </c>
       <c r="L72">
         <v>0.01</v>
@@ -4558,28 +4638,28 @@
       <c r="O72">
         <v>75</v>
       </c>
-      <c r="P72" s="11">
-        <v>0.1195</v>
+      <c r="P72" s="2">
+        <v>5.0500000000000003E-2</v>
       </c>
       <c r="Q72">
-        <v>29.520309999999998</v>
+        <v>3.9583469999999998</v>
       </c>
       <c r="R72">
-        <v>44.943669999999997</v>
+        <v>3.5701999999999998</v>
       </c>
       <c r="S72">
-        <v>25.20241</v>
+        <v>2.862905</v>
       </c>
       <c r="V72" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W72" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X72" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA72" t="str">
@@ -4595,19 +4675,19 @@
         <v>16</v>
       </c>
       <c r="C73">
-        <v>-5</v>
+        <v>-2.5</v>
       </c>
       <c r="D73">
         <v>-0.15</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="F73">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="G73">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="H73">
         <v>-0.3</v>
@@ -4616,10 +4696,10 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
       <c r="K73">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="L73">
         <v>0.01</v>
@@ -4633,32 +4713,32 @@
       <c r="O73">
         <v>75</v>
       </c>
-      <c r="P73" s="11">
-        <v>0.10199999999999999</v>
+      <c r="P73" s="2">
+        <v>0.108</v>
       </c>
       <c r="Q73">
-        <v>30.520879999999998</v>
+        <v>8.5242690000000003</v>
       </c>
       <c r="R73">
-        <v>29.405550000000002</v>
+        <v>12.167657</v>
       </c>
       <c r="S73">
-        <v>26.754809999999999</v>
+        <v>8.2206430000000008</v>
       </c>
       <c r="V73" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W73" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X73" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA73" t="str">
-        <f t="shared" ref="AA73:AA80" si="16">IF(M73=10000,IF(IF(P74="",P73,"")=0,"",IF(P74="",P73,"")),"")</f>
+        <f t="shared" ref="AA73:AA89" si="22">IF(M73=10000,IF(IF(P74="",P73,"")=0,"",IF(P74="",P73,"")),"")</f>
         <v/>
       </c>
     </row>
@@ -4670,142 +4750,256 @@
         <v>16</v>
       </c>
       <c r="C74">
-        <v>-5</v>
+        <v>-3.5</v>
       </c>
       <c r="D74">
         <v>-0.15</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F74">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="G74">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="H74">
+        <v>-0.3</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>0.01</v>
+      </c>
+      <c r="M74">
+        <v>2000</v>
+      </c>
+      <c r="N74">
+        <v>100</v>
+      </c>
+      <c r="O74">
+        <v>75</v>
+      </c>
+      <c r="P74" s="11">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="Q74">
+        <v>3.6942210000000002</v>
+      </c>
+      <c r="R74">
+        <v>5.7041209999999998</v>
+      </c>
+      <c r="S74">
+        <v>4.7920980000000002</v>
+      </c>
+      <c r="V74" t="b">
+        <f t="shared" ref="V74" si="23">IF(C74="","",IF(C74&gt;F74, IF(C74&lt;G74, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="W74" t="b">
+        <f t="shared" ref="W74" si="24">IF(D74="","",IF(D74&gt;H74, IF(D74&lt;I74, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X74" t="b">
+        <f t="shared" ref="X74" si="25">IF(E74="","",IF(E74&gt;J74, IF(E74&lt;K74, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA74" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75">
+        <v>-3.5</v>
+      </c>
+      <c r="D75">
+        <v>-0.15</v>
+      </c>
+      <c r="E75">
+        <v>0.5</v>
+      </c>
+      <c r="F75">
+        <v>-7</v>
+      </c>
+      <c r="G75">
+        <v>-2</v>
+      </c>
+      <c r="H75">
         <v>-0.5</v>
       </c>
-      <c r="I74">
-        <v>-0.05</v>
-      </c>
-      <c r="J74">
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>2</v>
+      </c>
+      <c r="L75">
+        <v>0.01</v>
+      </c>
+      <c r="M75">
+        <v>2000</v>
+      </c>
+      <c r="N75">
+        <v>100</v>
+      </c>
+      <c r="O75">
+        <v>75</v>
+      </c>
+      <c r="P75" s="11">
+        <v>7.6499999999999999E-2</v>
+      </c>
+      <c r="Q75">
+        <v>2.0420980000000002</v>
+      </c>
+      <c r="R75">
+        <v>8.7851730000000003</v>
+      </c>
+      <c r="S75">
+        <v>4.8587400000000001</v>
+      </c>
+      <c r="V75" t="b">
+        <f t="shared" ref="V75:V81" si="26">IF(C75="","",IF(C75&gt;F75, IF(C75&lt;G75, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="W75" t="b">
+        <f t="shared" ref="W75:W81" si="27">IF(D75="","",IF(D75&gt;H75, IF(D75&lt;I75, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X75" t="b">
+        <f t="shared" ref="X75:X81" si="28">IF(E75="","",IF(E75&gt;J75, IF(E75&lt;K75, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA75" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76">
+        <v>-5.5</v>
+      </c>
+      <c r="D76">
+        <v>-0.15</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>-9</v>
+      </c>
+      <c r="G76">
+        <v>-2</v>
+      </c>
+      <c r="H76">
+        <v>-0.5</v>
+      </c>
+      <c r="I76">
         <v>0.5</v>
       </c>
-      <c r="K74">
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
         <v>2</v>
       </c>
-      <c r="L74">
-        <v>0.01</v>
-      </c>
-      <c r="M74">
-        <v>10000</v>
-      </c>
-      <c r="N74">
-        <v>100</v>
-      </c>
-      <c r="O74">
-        <v>75</v>
-      </c>
-      <c r="P74" s="11">
-        <v>0.1069</v>
-      </c>
-      <c r="Q74">
-        <v>149.62569999999999</v>
-      </c>
-      <c r="R74">
-        <v>218.458</v>
-      </c>
-      <c r="S74">
-        <v>123.6705</v>
-      </c>
-      <c r="V74" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="W74" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="X74" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AA74">
-        <f t="shared" si="16"/>
-        <v>0.1069</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V75" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="W75" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="X75" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="AA75" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V76" t="str">
-        <f t="shared" ref="V76:V78" si="17">IF(C76="","",IF(C76&gt;F76, IF(C76&lt;G76, TRUE, FALSE), FALSE))</f>
-        <v/>
-      </c>
-      <c r="W76" t="str">
-        <f t="shared" ref="W76:W78" si="18">IF(D76="","",IF(D76&gt;H76, IF(D76&lt;I76, TRUE, FALSE), FALSE))</f>
-        <v/>
-      </c>
-      <c r="X76" t="str">
-        <f t="shared" ref="X76:X78" si="19">IF(E76="","",IF(E76&gt;J76, IF(E76&lt;K76, TRUE, FALSE), FALSE))</f>
-        <v/>
+      <c r="L76">
+        <v>0.01</v>
+      </c>
+      <c r="M76">
+        <v>2000</v>
+      </c>
+      <c r="N76">
+        <v>100</v>
+      </c>
+      <c r="O76">
+        <v>75</v>
+      </c>
+      <c r="P76" s="11">
+        <v>0.16350000000000001</v>
+      </c>
+      <c r="Q76">
+        <v>30.73854</v>
+      </c>
+      <c r="R76">
+        <v>47.048760000000001</v>
+      </c>
+      <c r="S76">
+        <v>19.026399999999999</v>
+      </c>
+      <c r="V76" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="W76" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="X76" t="b">
+        <f t="shared" si="28"/>
+        <v>1</v>
       </c>
       <c r="AA76" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B77" t="s">
         <v>16</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>-0.15</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="G77">
-        <v>5</v>
+        <v>-4</v>
       </c>
       <c r="H77">
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="I77">
-        <v>0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="J77">
-        <v>-0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K77">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="L77">
         <v>0.01</v>
@@ -4819,68 +5013,68 @@
       <c r="O77">
         <v>75</v>
       </c>
-      <c r="P77" s="2">
-        <v>6.1499999999999999E-2</v>
+      <c r="P77" s="11">
+        <v>0.13450000000000001</v>
       </c>
       <c r="Q77">
-        <v>2.3140849999999999</v>
+        <v>8.1231609999999996</v>
       </c>
       <c r="R77">
-        <v>7.3612200000000003</v>
+        <v>27.910938999999999</v>
       </c>
       <c r="S77">
-        <v>2.1175869999999999</v>
+        <v>16.052879000000001</v>
       </c>
       <c r="V77" t="b">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="W77" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="X77" t="b">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="AA77" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
       </c>
       <c r="C78">
-        <v>-1.5</v>
+        <v>-5</v>
       </c>
       <c r="D78">
-        <v>0.1</v>
+        <v>-0.15</v>
       </c>
       <c r="E78">
-        <v>-0.4</v>
+        <v>1</v>
       </c>
       <c r="F78">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="H78">
-        <v>-0.2</v>
+        <v>-0.25</v>
       </c>
       <c r="I78">
-        <v>0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="J78">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="K78">
-        <v>0.2</v>
+        <v>1.25</v>
       </c>
       <c r="L78">
         <v>0.01</v>
@@ -4894,68 +5088,68 @@
       <c r="O78">
         <v>75</v>
       </c>
-      <c r="P78" s="2">
-        <v>6.6500000000000004E-2</v>
+      <c r="P78" s="11">
+        <v>0.1195</v>
       </c>
       <c r="Q78">
-        <v>1.825928</v>
+        <v>29.520309999999998</v>
       </c>
       <c r="R78">
-        <v>63.439382000000002</v>
+        <v>44.943669999999997</v>
       </c>
       <c r="S78">
-        <v>1.4714320000000001</v>
+        <v>25.20241</v>
       </c>
       <c r="V78" t="b">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="W78" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="X78" t="b">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="AA78" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
       </c>
       <c r="C79">
-        <v>-1.5</v>
+        <v>-5</v>
       </c>
       <c r="D79">
-        <v>-2.5000000000000001E-2</v>
+        <v>-0.15</v>
       </c>
       <c r="E79">
-        <v>-0.4</v>
+        <v>1</v>
       </c>
       <c r="F79">
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="G79">
-        <v>0.5</v>
+        <v>-4</v>
       </c>
       <c r="H79">
-        <v>-0.05</v>
+        <v>-0.3</v>
       </c>
       <c r="I79">
         <v>0</v>
       </c>
       <c r="J79">
-        <v>-2</v>
+        <v>0.75</v>
       </c>
       <c r="K79">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L79">
         <v>0.01</v>
@@ -4969,108 +5163,669 @@
       <c r="O79">
         <v>75</v>
       </c>
-      <c r="P79" s="2">
-        <v>8.0500000000000002E-2</v>
+      <c r="P79" s="11">
+        <v>0.10199999999999999</v>
       </c>
       <c r="Q79">
-        <v>4.5501940000000003</v>
+        <v>30.520879999999998</v>
       </c>
       <c r="R79">
-        <v>6.3748089999999999</v>
+        <v>29.405550000000002</v>
       </c>
       <c r="S79">
-        <v>3.5062099999999998</v>
+        <v>26.754809999999999</v>
       </c>
       <c r="V79" t="b">
-        <f t="shared" ref="V79:V80" si="20">IF(C79="","",IF(C79&gt;F79, IF(C79&lt;G79, TRUE, FALSE), FALSE))</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="W79" t="b">
-        <f t="shared" ref="W79:W80" si="21">IF(D79="","",IF(D79&gt;H79, IF(D79&lt;I79, TRUE, FALSE), FALSE))</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="X79" t="b">
-        <f t="shared" ref="X79:X80" si="22">IF(E79="","",IF(E79&gt;J79, IF(E79&lt;K79, TRUE, FALSE), FALSE))</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="AA79" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80">
+        <v>-5</v>
+      </c>
+      <c r="D80">
+        <v>-0.15</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>-6</v>
+      </c>
+      <c r="G80">
+        <v>-4</v>
+      </c>
+      <c r="H80">
+        <v>-0.5</v>
+      </c>
+      <c r="I80">
+        <v>-0.05</v>
+      </c>
+      <c r="J80">
+        <v>0.5</v>
+      </c>
+      <c r="K80">
+        <v>2</v>
+      </c>
+      <c r="L80">
+        <v>0.01</v>
+      </c>
+      <c r="M80">
+        <v>10000</v>
+      </c>
+      <c r="N80">
+        <v>100</v>
+      </c>
+      <c r="O80">
+        <v>75</v>
+      </c>
+      <c r="P80" s="11">
+        <v>0.1069</v>
+      </c>
+      <c r="Q80">
+        <v>149.62569999999999</v>
+      </c>
+      <c r="R80">
+        <v>218.458</v>
+      </c>
+      <c r="S80">
+        <v>123.6705</v>
+      </c>
+      <c r="V80" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="W80" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="X80" t="b">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="AA80">
+        <f t="shared" si="22"/>
+        <v>0.1069</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="V81" t="str">
+        <f t="shared" si="26"/>
+        <v/>
+      </c>
+      <c r="W81" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="X81" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AA81" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="V82" t="str">
+        <f t="shared" ref="V82:V84" si="29">IF(C82="","",IF(C82&gt;F82, IF(C82&lt;G82, TRUE, FALSE), FALSE))</f>
+        <v/>
+      </c>
+      <c r="W82" t="str">
+        <f t="shared" ref="W82:W84" si="30">IF(D82="","",IF(D82&gt;H82, IF(D82&lt;I82, TRUE, FALSE), FALSE))</f>
+        <v/>
+      </c>
+      <c r="X82" t="str">
+        <f t="shared" ref="X82:X84" si="31">IF(E82="","",IF(E82&gt;J82, IF(E82&lt;K82, TRUE, FALSE), FALSE))</f>
+        <v/>
+      </c>
+      <c r="AA82" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>28</v>
       </c>
-      <c r="B80" t="s">
-        <v>16</v>
-      </c>
-      <c r="C80">
+      <c r="B83" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>-5</v>
+      </c>
+      <c r="G83">
+        <v>5</v>
+      </c>
+      <c r="H83">
+        <v>-0.1</v>
+      </c>
+      <c r="I83">
+        <v>0.1</v>
+      </c>
+      <c r="J83">
+        <v>-0.1</v>
+      </c>
+      <c r="K83">
+        <v>0.1</v>
+      </c>
+      <c r="L83">
+        <v>0.01</v>
+      </c>
+      <c r="M83">
+        <v>2000</v>
+      </c>
+      <c r="N83">
+        <v>100</v>
+      </c>
+      <c r="O83">
+        <v>75</v>
+      </c>
+      <c r="P83" s="2">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="Q83">
+        <v>2.3140849999999999</v>
+      </c>
+      <c r="R83">
+        <v>7.3612200000000003</v>
+      </c>
+      <c r="S83">
+        <v>2.1175869999999999</v>
+      </c>
+      <c r="V83" t="b">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="W83" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="X83" t="b">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="AA83" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84">
+        <v>-1.5</v>
+      </c>
+      <c r="D84">
+        <v>0.1</v>
+      </c>
+      <c r="E84">
+        <v>-0.4</v>
+      </c>
+      <c r="F84">
+        <v>-3</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>-0.2</v>
+      </c>
+      <c r="I84">
+        <v>0.5</v>
+      </c>
+      <c r="J84">
         <v>-1</v>
       </c>
-      <c r="D80">
+      <c r="K84">
+        <v>0.2</v>
+      </c>
+      <c r="L84">
+        <v>0.01</v>
+      </c>
+      <c r="M84">
+        <v>2000</v>
+      </c>
+      <c r="N84">
+        <v>100</v>
+      </c>
+      <c r="O84">
+        <v>75</v>
+      </c>
+      <c r="P84" s="2">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="Q84">
+        <v>1.825928</v>
+      </c>
+      <c r="R84">
+        <v>63.439382000000002</v>
+      </c>
+      <c r="S84">
+        <v>1.4714320000000001</v>
+      </c>
+      <c r="V84" t="b">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="W84" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="X84" t="b">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="AA84" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85">
+        <v>-1.5</v>
+      </c>
+      <c r="D85">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="E85">
+        <v>-0.4</v>
+      </c>
+      <c r="F85">
+        <v>-2</v>
+      </c>
+      <c r="G85">
+        <v>0.5</v>
+      </c>
+      <c r="H85">
+        <v>-0.05</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>-2</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0.01</v>
+      </c>
+      <c r="M85">
+        <v>2000</v>
+      </c>
+      <c r="N85">
+        <v>100</v>
+      </c>
+      <c r="O85">
+        <v>75</v>
+      </c>
+      <c r="P85" s="2">
+        <v>8.0500000000000002E-2</v>
+      </c>
+      <c r="Q85">
+        <v>4.5501940000000003</v>
+      </c>
+      <c r="R85">
+        <v>6.3748089999999999</v>
+      </c>
+      <c r="S85">
+        <v>3.5062099999999998</v>
+      </c>
+      <c r="V85" t="b">
+        <f t="shared" ref="V85:V87" si="32">IF(C85="","",IF(C85&gt;F85, IF(C85&lt;G85, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="W85" t="b">
+        <f t="shared" ref="W85:W87" si="33">IF(D85="","",IF(D85&gt;H85, IF(D85&lt;I85, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X85" t="b">
+        <f t="shared" ref="X85:X87" si="34">IF(E85="","",IF(E85&gt;J85, IF(E85&lt;K85, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA85" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86">
+        <v>-1</v>
+      </c>
+      <c r="D86">
         <v>-0.25</v>
       </c>
-      <c r="E80">
+      <c r="E86">
         <v>-0.5</v>
       </c>
-      <c r="F80">
+      <c r="F86">
         <v>-2</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
         <v>-0.75</v>
       </c>
-      <c r="I80">
+      <c r="I86">
         <v>0.25</v>
       </c>
-      <c r="J80">
+      <c r="J86">
         <v>-1</v>
       </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-      <c r="L80">
-        <v>0.01</v>
-      </c>
-      <c r="M80">
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0.01</v>
+      </c>
+      <c r="M86">
         <v>2000</v>
       </c>
-      <c r="N80">
-        <v>100</v>
-      </c>
-      <c r="O80">
-        <v>75</v>
-      </c>
-      <c r="P80" s="2">
+      <c r="N86">
+        <v>100</v>
+      </c>
+      <c r="O86">
+        <v>75</v>
+      </c>
+      <c r="P86" s="2">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="Q80">
+      <c r="Q86">
         <v>14.898250000000001</v>
       </c>
-      <c r="R80">
+      <c r="R86">
         <v>61.730719999999998</v>
       </c>
-      <c r="S80">
+      <c r="S86">
         <v>14.133800000000001</v>
       </c>
-      <c r="V80" t="b">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="W80" t="b">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-      <c r="X80" t="b">
+      <c r="V86" t="b">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="W86" t="b">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="X86" t="b">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="AA86" t="str">
         <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-      <c r="AA80" t="str">
-        <f t="shared" si="16"/>
-        <v/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87">
+        <v>-0.5</v>
+      </c>
+      <c r="D87">
+        <v>-0.3</v>
+      </c>
+      <c r="E87">
+        <v>-0.75</v>
+      </c>
+      <c r="F87">
+        <v>-1.5</v>
+      </c>
+      <c r="G87">
+        <v>0.5</v>
+      </c>
+      <c r="H87">
+        <v>-0.75</v>
+      </c>
+      <c r="I87">
+        <v>0.1</v>
+      </c>
+      <c r="J87">
+        <v>-1.5</v>
+      </c>
+      <c r="K87">
+        <v>-0.1</v>
+      </c>
+      <c r="L87">
+        <v>0.01</v>
+      </c>
+      <c r="M87">
+        <v>2000</v>
+      </c>
+      <c r="N87">
+        <v>100</v>
+      </c>
+      <c r="O87">
+        <v>75</v>
+      </c>
+      <c r="P87" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="Q87">
+        <v>9.1500129999999995</v>
+      </c>
+      <c r="R87">
+        <v>23.194382000000001</v>
+      </c>
+      <c r="S87">
+        <v>6.2325189999999999</v>
+      </c>
+      <c r="V87" t="b">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="W87" t="b">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="X87" t="b">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="AA87" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88">
+        <v>-0.5</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>-0.75</v>
+      </c>
+      <c r="F88">
+        <v>-1</v>
+      </c>
+      <c r="G88">
+        <v>-0.2</v>
+      </c>
+      <c r="H88">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="I88">
+        <v>0.1</v>
+      </c>
+      <c r="J88">
+        <v>-1</v>
+      </c>
+      <c r="K88">
+        <v>-0.5</v>
+      </c>
+      <c r="L88">
+        <v>0.01</v>
+      </c>
+      <c r="M88">
+        <v>2000</v>
+      </c>
+      <c r="N88">
+        <v>100</v>
+      </c>
+      <c r="O88">
+        <v>75</v>
+      </c>
+      <c r="P88" s="2">
+        <v>0.224</v>
+      </c>
+      <c r="Q88">
+        <v>44.817950000000003</v>
+      </c>
+      <c r="R88">
+        <v>43.052370000000003</v>
+      </c>
+      <c r="S88">
+        <v>44.186599999999999</v>
+      </c>
+      <c r="V88" t="b">
+        <f t="shared" ref="V88" si="35">IF(C88="","",IF(C88&gt;F88, IF(C88&lt;G88, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="W88" t="b">
+        <f t="shared" ref="W88" si="36">IF(D88="","",IF(D88&gt;H88, IF(D88&lt;I88, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X88" t="b">
+        <f t="shared" ref="X88" si="37">IF(E88="","",IF(E88&gt;J88, IF(E88&lt;K88, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA88" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89">
+        <v>-0.5</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>-0.75</v>
+      </c>
+      <c r="F89">
+        <v>-1</v>
+      </c>
+      <c r="G89">
+        <v>-0.2</v>
+      </c>
+      <c r="H89">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="I89">
+        <v>0.1</v>
+      </c>
+      <c r="J89">
+        <v>-1</v>
+      </c>
+      <c r="K89">
+        <v>-0.5</v>
+      </c>
+      <c r="L89">
+        <v>0.01</v>
+      </c>
+      <c r="M89">
+        <v>10000</v>
+      </c>
+      <c r="N89">
+        <v>100</v>
+      </c>
+      <c r="O89">
+        <v>75</v>
+      </c>
+      <c r="P89" s="2">
+        <v>0.14369999999999999</v>
+      </c>
+      <c r="Q89">
+        <v>128.5677</v>
+      </c>
+      <c r="R89">
+        <v>424.99579999999997</v>
+      </c>
+      <c r="S89">
+        <v>123.0753</v>
+      </c>
+      <c r="V89" t="b">
+        <f t="shared" ref="V89" si="38">IF(C89="","",IF(C89&gt;F89, IF(C89&lt;G89, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="W89" t="b">
+        <f t="shared" ref="W89" si="39">IF(D89="","",IF(D89&gt;H89, IF(D89&lt;I89, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="X89" t="b">
+        <f t="shared" ref="X89" si="40">IF(E89="","",IF(E89&gt;J89, IF(E89&lt;K89, TRUE, FALSE), FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="AA89">
+        <f t="shared" si="22"/>
+        <v>0.14369999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5083,7 +5838,7 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="V1:X6 V7 V8:X1048576 AA6">
+  <conditionalFormatting sqref="V1:X6 V7 AA6 V8:X1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>

</xml_diff>